<commit_message>
finalise Table of compounds to account for duplicated Controls and generate Heatmaps
</commit_message>
<xml_diff>
--- a/data/Table of compounds.xlsx
+++ b/data/Table of compounds.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="671" documentId="11_C9C3E2DFE6E5ECF5CE906EFDC2549BB3DEDA2518" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C2B03F7-E109-42B6-83E5-AC95858A8635}"/>
+  <xr:revisionPtr revIDLastSave="687" documentId="11_C9C3E2DFE6E5ECF5CE906EFDC2549BB3DEDA2518" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{246463A5-2364-4429-A370-CB10D9D5C3C2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="380" windowWidth="19200" windowHeight="10310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="490" windowWidth="19200" windowHeight="10310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experimental Design" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="557">
   <si>
     <t>Samples</t>
   </si>
@@ -1756,6 +1756,9 @@
   </si>
   <si>
     <t>021222</t>
+  </si>
+  <si>
+    <t>Dose Response</t>
   </si>
 </sst>
 </file>
@@ -2974,7 +2977,6 @@
     <xf numFmtId="49" fontId="0" fillId="11" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3221,6 +3223,27 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3230,28 +3253,73 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="10" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3273,48 +3341,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3341,6 +3367,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3389,87 +3421,58 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3933,8 +3936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -3981,13 +3984,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="288" t="s">
+      <c r="A2" s="294" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="323" t="s">
+      <c r="B2" s="330" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="326"/>
+      <c r="C2" s="333"/>
       <c r="D2" s="4">
         <v>2</v>
       </c>
@@ -4007,9 +4010,9 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="289"/>
-      <c r="B3" s="324"/>
-      <c r="C3" s="327"/>
+      <c r="A3" s="295"/>
+      <c r="B3" s="331"/>
+      <c r="C3" s="334"/>
       <c r="D3" s="4">
         <v>2</v>
       </c>
@@ -4029,9 +4032,9 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="289"/>
-      <c r="B4" s="324"/>
-      <c r="C4" s="327"/>
+      <c r="A4" s="295"/>
+      <c r="B4" s="331"/>
+      <c r="C4" s="334"/>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
@@ -4051,9 +4054,9 @@
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="289"/>
-      <c r="B5" s="324"/>
-      <c r="C5" s="327"/>
+      <c r="A5" s="295"/>
+      <c r="B5" s="331"/>
+      <c r="C5" s="334"/>
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
@@ -4073,9 +4076,9 @@
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="289"/>
-      <c r="B6" s="324"/>
-      <c r="C6" s="327"/>
+      <c r="A6" s="295"/>
+      <c r="B6" s="331"/>
+      <c r="C6" s="334"/>
       <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
@@ -4095,9 +4098,9 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="289"/>
-      <c r="B7" s="324"/>
-      <c r="C7" s="327"/>
+      <c r="A7" s="295"/>
+      <c r="B7" s="331"/>
+      <c r="C7" s="334"/>
       <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
@@ -4117,11 +4120,11 @@
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="289"/>
-      <c r="B8" s="324"/>
-      <c r="C8" s="327"/>
-      <c r="D8" s="286"/>
-      <c r="E8" s="286"/>
+      <c r="A8" s="295"/>
+      <c r="B8" s="331"/>
+      <c r="C8" s="334"/>
+      <c r="D8" s="285"/>
+      <c r="E8" s="285"/>
       <c r="F8" t="s">
         <v>15</v>
       </c>
@@ -4139,9 +4142,9 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="289"/>
-      <c r="B9" s="324"/>
-      <c r="C9" s="328"/>
+      <c r="A9" s="295"/>
+      <c r="B9" s="331"/>
+      <c r="C9" s="335"/>
       <c r="D9" t="s">
         <v>13</v>
       </c>
@@ -4162,13 +4165,13 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="289"/>
-      <c r="B10" s="324"/>
-      <c r="C10" s="328"/>
-      <c r="D10" s="203" t="s">
+      <c r="A10" s="295"/>
+      <c r="B10" s="331"/>
+      <c r="C10" s="335"/>
+      <c r="D10" s="202" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="206"/>
+      <c r="E10" s="205"/>
       <c r="F10" s="140" t="s">
         <v>196</v>
       </c>
@@ -4181,20 +4184,20 @@
       <c r="I10" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="J10" s="204"/>
+      <c r="J10" s="203"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="289"/>
-      <c r="B11" s="325"/>
-      <c r="C11" s="329"/>
-      <c r="D11" s="202" t="s">
+      <c r="A11" s="295"/>
+      <c r="B11" s="332"/>
+      <c r="C11" s="336"/>
+      <c r="D11" s="201" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="207"/>
-      <c r="F11" s="202" t="s">
+      <c r="E11" s="206"/>
+      <c r="F11" s="201" t="s">
         <v>228</v>
       </c>
-      <c r="G11" s="202" t="s">
+      <c r="G11" s="201" t="s">
         <v>254</v>
       </c>
       <c r="H11" t="s">
@@ -4203,14 +4206,14 @@
       <c r="I11" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="J11" s="205"/>
+      <c r="J11" s="204"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="289"/>
-      <c r="B12" s="343" t="s">
+      <c r="A12" s="295"/>
+      <c r="B12" s="352" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="326"/>
+      <c r="C12" s="333"/>
       <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
@@ -4230,9 +4233,9 @@
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="289"/>
-      <c r="B13" s="344"/>
-      <c r="C13" s="340"/>
+      <c r="A13" s="295"/>
+      <c r="B13" s="353"/>
+      <c r="C13" s="349"/>
       <c r="D13" s="5" t="s">
         <v>18</v>
       </c>
@@ -4252,20 +4255,20 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="289"/>
-      <c r="B14" s="344"/>
-      <c r="C14" s="340"/>
+      <c r="A14" s="295"/>
+      <c r="B14" s="353"/>
+      <c r="C14" s="349"/>
       <c r="D14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="372" t="s">
         <v>546</v>
       </c>
       <c r="I14" s="9" t="s">
@@ -4274,15 +4277,15 @@
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="289"/>
-      <c r="B15" s="344"/>
-      <c r="C15" s="340"/>
+      <c r="A15" s="295"/>
+      <c r="B15" s="353"/>
+      <c r="C15" s="349"/>
       <c r="D15" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>9</v>
@@ -4296,40 +4299,40 @@
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="289"/>
-      <c r="B16" s="344"/>
-      <c r="C16" s="340"/>
+      <c r="A16" s="295"/>
+      <c r="B16" s="353"/>
+      <c r="C16" s="349"/>
       <c r="D16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="H16" t="s">
         <v>546</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="289"/>
-      <c r="B17" s="344"/>
-      <c r="C17" s="340"/>
+      <c r="A17" s="295"/>
+      <c r="B17" s="353"/>
+      <c r="C17" s="349"/>
       <c r="D17" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="H17" t="s">
         <v>546</v>
@@ -4340,9 +4343,9 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="289"/>
-      <c r="B18" s="344"/>
-      <c r="C18" s="341"/>
+      <c r="A18" s="295"/>
+      <c r="B18" s="353"/>
+      <c r="C18" s="350"/>
       <c r="D18" s="12" t="s">
         <v>18</v>
       </c>
@@ -4362,9 +4365,9 @@
       <c r="J18" s="13"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="289"/>
-      <c r="B19" s="344"/>
-      <c r="C19" s="341"/>
+      <c r="A19" s="295"/>
+      <c r="B19" s="353"/>
+      <c r="C19" s="350"/>
       <c r="D19" t="s">
         <v>18</v>
       </c>
@@ -4380,12 +4383,12 @@
       <c r="I19" t="s">
         <v>543</v>
       </c>
-      <c r="J19" s="285"/>
+      <c r="J19" s="284"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="289"/>
-      <c r="B20" s="344"/>
-      <c r="C20" s="341"/>
+      <c r="A20" s="295"/>
+      <c r="B20" s="353"/>
+      <c r="C20" s="350"/>
       <c r="D20" s="24" t="s">
         <v>18</v>
       </c>
@@ -4405,9 +4408,9 @@
       <c r="J20" s="142"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="289"/>
-      <c r="B21" s="344"/>
-      <c r="C21" s="341"/>
+      <c r="A21" s="295"/>
+      <c r="B21" s="353"/>
+      <c r="C21" s="350"/>
       <c r="D21" s="141" t="s">
         <v>18</v>
       </c>
@@ -4427,9 +4430,9 @@
       <c r="J21" s="143"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="289"/>
-      <c r="B22" s="344"/>
-      <c r="C22" s="341"/>
+      <c r="A22" s="295"/>
+      <c r="B22" s="353"/>
+      <c r="C22" s="350"/>
       <c r="D22" s="120" t="s">
         <v>19</v>
       </c>
@@ -4451,9 +4454,9 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="289"/>
-      <c r="B23" s="344"/>
-      <c r="C23" s="342"/>
+      <c r="A23" s="295"/>
+      <c r="B23" s="353"/>
+      <c r="C23" s="351"/>
       <c r="D23" s="21" t="s">
         <v>18</v>
       </c>
@@ -4473,17 +4476,17 @@
       <c r="J23" s="142"/>
     </row>
     <row r="24" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="289"/>
-      <c r="B24" s="344"/>
-      <c r="C24" s="274"/>
-      <c r="D24" s="275" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="276"/>
-      <c r="F24" s="275" t="s">
+      <c r="A24" s="295"/>
+      <c r="B24" s="353"/>
+      <c r="C24" s="273"/>
+      <c r="D24" s="274" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="275"/>
+      <c r="F24" s="274" t="s">
         <v>532</v>
       </c>
-      <c r="G24" s="275" t="s">
+      <c r="G24" s="274" t="s">
         <v>534</v>
       </c>
       <c r="H24" t="s">
@@ -4492,18 +4495,18 @@
       <c r="I24" s="9" t="s">
         <v>543</v>
       </c>
-      <c r="J24" s="277" t="s">
+      <c r="J24" s="276" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="289"/>
-      <c r="B25" s="344"/>
-      <c r="C25" s="274"/>
-      <c r="D25" s="275" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="276"/>
+      <c r="A25" s="295"/>
+      <c r="B25" s="353"/>
+      <c r="C25" s="273"/>
+      <c r="D25" s="274" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="275"/>
       <c r="F25" s="21" t="s">
         <v>532</v>
       </c>
@@ -4516,18 +4519,18 @@
       <c r="I25" s="9" t="s">
         <v>542</v>
       </c>
-      <c r="J25" s="277" t="s">
+      <c r="J25" s="276" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="289"/>
-      <c r="B26" s="344"/>
-      <c r="C26" s="274"/>
-      <c r="D26" s="275" t="s">
+      <c r="A26" s="295"/>
+      <c r="B26" s="353"/>
+      <c r="C26" s="273"/>
+      <c r="D26" s="274" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="276"/>
+      <c r="E26" s="275"/>
       <c r="F26" s="21" t="s">
         <v>532</v>
       </c>
@@ -4540,18 +4543,18 @@
       <c r="I26" s="9" t="s">
         <v>542</v>
       </c>
-      <c r="J26" s="277" t="s">
+      <c r="J26" s="276" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="290"/>
-      <c r="B27" s="345"/>
-      <c r="C27" s="274"/>
-      <c r="D27" s="275" t="s">
+      <c r="A27" s="296"/>
+      <c r="B27" s="354"/>
+      <c r="C27" s="273"/>
+      <c r="D27" s="274" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="276"/>
+      <c r="E27" s="275"/>
       <c r="F27" s="21" t="s">
         <v>532</v>
       </c>
@@ -4564,18 +4567,18 @@
       <c r="I27" s="9" t="s">
         <v>542</v>
       </c>
-      <c r="J27" s="277" t="s">
+      <c r="J27" s="276" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="333" t="s">
+      <c r="A28" s="342" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="291" t="s">
+      <c r="B28" s="337" t="s">
         <v>143</v>
       </c>
-      <c r="C28" s="337" t="s">
+      <c r="C28" s="346" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="122" t="s">
@@ -4601,13 +4604,13 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="334"/>
-      <c r="B29" s="292"/>
-      <c r="C29" s="338"/>
+      <c r="A29" s="343"/>
+      <c r="B29" s="358"/>
+      <c r="C29" s="347"/>
       <c r="D29" s="124" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="190" t="s">
+      <c r="E29" s="189" t="s">
         <v>56</v>
       </c>
       <c r="F29" s="125" t="s">
@@ -4625,13 +4628,13 @@
       <c r="J29" s="126"/>
     </row>
     <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="334"/>
-      <c r="B30" s="292"/>
-      <c r="C30" s="338"/>
+      <c r="A30" s="343"/>
+      <c r="B30" s="358"/>
+      <c r="C30" s="347"/>
       <c r="D30" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="190" t="s">
+      <c r="E30" s="189" t="s">
         <v>56</v>
       </c>
       <c r="F30" s="125" t="s">
@@ -4649,13 +4652,13 @@
       <c r="J30" s="128"/>
     </row>
     <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="334"/>
-      <c r="B31" s="292"/>
-      <c r="C31" s="338"/>
+      <c r="A31" s="343"/>
+      <c r="B31" s="358"/>
+      <c r="C31" s="347"/>
       <c r="D31" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="E31" s="190" t="s">
+      <c r="E31" s="189" t="s">
         <v>56</v>
       </c>
       <c r="F31" s="129" t="s">
@@ -4673,9 +4676,9 @@
       <c r="J31" s="128"/>
     </row>
     <row r="32" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="334"/>
-      <c r="B32" s="292"/>
-      <c r="C32" s="338"/>
+      <c r="A32" s="343"/>
+      <c r="B32" s="358"/>
+      <c r="C32" s="347"/>
       <c r="D32" s="127" t="s">
         <v>18</v>
       </c>
@@ -4694,16 +4697,18 @@
       <c r="I32" s="125" t="s">
         <v>543</v>
       </c>
-      <c r="J32" s="128"/>
+      <c r="J32" s="128" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="334"/>
-      <c r="B33" s="292"/>
-      <c r="C33" s="338"/>
+      <c r="A33" s="343"/>
+      <c r="B33" s="358"/>
+      <c r="C33" s="347"/>
       <c r="D33" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="190" t="s">
+      <c r="E33" s="189" t="s">
         <v>56</v>
       </c>
       <c r="F33" s="129" t="s">
@@ -4718,12 +4723,14 @@
       <c r="I33" s="125" t="s">
         <v>543</v>
       </c>
-      <c r="J33" s="128"/>
+      <c r="J33" s="128" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="34" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="334"/>
-      <c r="B34" s="292"/>
-      <c r="C34" s="338"/>
+      <c r="A34" s="343"/>
+      <c r="B34" s="358"/>
+      <c r="C34" s="347"/>
       <c r="D34" s="127" t="s">
         <v>18</v>
       </c>
@@ -4742,12 +4749,14 @@
       <c r="I34" s="125" t="s">
         <v>543</v>
       </c>
-      <c r="J34" s="128"/>
+      <c r="J34" s="128" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="334"/>
-      <c r="B35" s="292"/>
-      <c r="C35" s="338"/>
+      <c r="A35" s="343"/>
+      <c r="B35" s="358"/>
+      <c r="C35" s="347"/>
       <c r="D35" s="165" t="s">
         <v>18</v>
       </c>
@@ -4766,202 +4775,204 @@
       <c r="I35" s="125" t="s">
         <v>543</v>
       </c>
-      <c r="J35" s="167"/>
+      <c r="J35" s="128" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="334"/>
-      <c r="B36" s="292"/>
-      <c r="C36" s="338"/>
+      <c r="A36" s="343"/>
+      <c r="B36" s="358"/>
+      <c r="C36" s="347"/>
       <c r="D36" s="165" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="190" t="s">
+      <c r="E36" s="189" t="s">
         <v>56</v>
       </c>
-      <c r="F36" s="190" t="s">
+      <c r="F36" s="189" t="s">
         <v>532</v>
       </c>
       <c r="G36" s="164" t="s">
         <v>534</v>
       </c>
-      <c r="H36" s="281" t="s">
+      <c r="H36" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I36" s="125" t="s">
         <v>543</v>
       </c>
-      <c r="J36" s="192" t="s">
+      <c r="J36" s="191" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="334"/>
-      <c r="B37" s="292"/>
-      <c r="C37" s="338"/>
+      <c r="A37" s="343"/>
+      <c r="B37" s="358"/>
+      <c r="C37" s="347"/>
       <c r="D37" s="165" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="190" t="s">
+      <c r="E37" s="189" t="s">
         <v>56</v>
       </c>
-      <c r="F37" s="190" t="s">
+      <c r="F37" s="189" t="s">
         <v>536</v>
       </c>
       <c r="G37" s="164" t="s">
         <v>534</v>
       </c>
-      <c r="H37" s="281" t="s">
+      <c r="H37" s="280" t="s">
         <v>547</v>
       </c>
       <c r="I37" s="125" t="s">
         <v>543</v>
       </c>
-      <c r="J37" s="192" t="s">
+      <c r="J37" s="191" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="334"/>
-      <c r="B38" s="292"/>
-      <c r="C38" s="338"/>
+      <c r="A38" s="343"/>
+      <c r="B38" s="358"/>
+      <c r="C38" s="347"/>
       <c r="D38" s="165" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="190" t="s">
+      <c r="E38" s="189" t="s">
         <v>56</v>
       </c>
-      <c r="F38" s="190" t="s">
+      <c r="F38" s="189" t="s">
         <v>537</v>
       </c>
       <c r="G38" s="164" t="s">
         <v>534</v>
       </c>
-      <c r="H38" s="281" t="s">
+      <c r="H38" s="280" t="s">
         <v>548</v>
       </c>
       <c r="I38" s="125" t="s">
         <v>543</v>
       </c>
-      <c r="J38" s="192" t="s">
+      <c r="J38" s="191" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="334"/>
-      <c r="B39" s="292"/>
-      <c r="C39" s="338"/>
+      <c r="A39" s="343"/>
+      <c r="B39" s="358"/>
+      <c r="C39" s="347"/>
       <c r="D39" s="165" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="190" t="s">
+      <c r="E39" s="189" t="s">
         <v>56</v>
       </c>
-      <c r="F39" s="190" t="s">
+      <c r="F39" s="189" t="s">
         <v>555</v>
       </c>
       <c r="G39" s="164" t="s">
         <v>534</v>
       </c>
-      <c r="H39" s="281" t="s">
+      <c r="H39" s="280" t="s">
         <v>549</v>
       </c>
       <c r="I39" s="125" t="s">
         <v>543</v>
       </c>
-      <c r="J39" s="192" t="s">
+      <c r="J39" s="191" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="334"/>
-      <c r="B40" s="292"/>
-      <c r="C40" s="338"/>
+      <c r="A40" s="343"/>
+      <c r="B40" s="358"/>
+      <c r="C40" s="347"/>
       <c r="D40" s="165" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="190" t="s">
+      <c r="E40" s="189" t="s">
         <v>56</v>
       </c>
-      <c r="F40" s="190" t="s">
+      <c r="F40" s="189" t="s">
         <v>538</v>
       </c>
       <c r="G40" s="164" t="s">
         <v>534</v>
       </c>
-      <c r="H40" s="281" t="s">
+      <c r="H40" s="280" t="s">
         <v>550</v>
       </c>
       <c r="I40" s="125" t="s">
         <v>543</v>
       </c>
-      <c r="J40" s="192" t="s">
+      <c r="J40" s="191" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="334"/>
-      <c r="B41" s="292"/>
-      <c r="C41" s="339"/>
+      <c r="A41" s="343"/>
+      <c r="B41" s="358"/>
+      <c r="C41" s="348"/>
       <c r="D41" s="165" t="s">
         <v>73</v>
       </c>
-      <c r="E41" s="190" t="s">
+      <c r="E41" s="189" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="190" t="s">
+      <c r="F41" s="189" t="s">
         <v>540</v>
       </c>
       <c r="G41" s="164" t="s">
         <v>534</v>
       </c>
-      <c r="H41" s="281" t="s">
+      <c r="H41" s="280" t="s">
         <v>551</v>
       </c>
       <c r="I41" s="125" t="s">
         <v>543</v>
       </c>
-      <c r="J41" s="192" t="s">
+      <c r="J41" s="191" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="334"/>
-      <c r="B42" s="292"/>
+      <c r="A42" s="343"/>
+      <c r="B42" s="358"/>
       <c r="C42" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="189" t="s">
-        <v>18</v>
-      </c>
-      <c r="E42" s="190" t="s">
+      <c r="D42" s="188" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" s="189" t="s">
         <v>28</v>
       </c>
-      <c r="F42" s="190" t="s">
+      <c r="F42" s="189" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="189" t="s">
+      <c r="G42" s="188" t="s">
         <v>34</v>
       </c>
-      <c r="H42" s="281" t="s">
+      <c r="H42" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I42" s="163" t="s">
         <v>543</v>
       </c>
-      <c r="J42" s="192" t="s">
+      <c r="J42" s="191" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="334"/>
-      <c r="B43" s="292"/>
-      <c r="C43" s="187" t="s">
+      <c r="A43" s="343"/>
+      <c r="B43" s="358"/>
+      <c r="C43" s="186" t="s">
         <v>211</v>
       </c>
-      <c r="D43" s="189" t="s">
-        <v>18</v>
-      </c>
-      <c r="E43" s="189" t="s">
+      <c r="D43" s="188" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="188" t="s">
         <v>214</v>
       </c>
       <c r="F43" s="131" t="s">
@@ -4970,98 +4981,98 @@
       <c r="G43" s="131" t="s">
         <v>197</v>
       </c>
-      <c r="H43" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I43" s="280" t="s">
+      <c r="H43" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I43" s="279" t="s">
         <v>543</v>
       </c>
-      <c r="J43" s="193"/>
+      <c r="J43" s="192"/>
     </row>
     <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="334"/>
-      <c r="B44" s="292"/>
-      <c r="C44" s="187" t="s">
+      <c r="A44" s="343"/>
+      <c r="B44" s="358"/>
+      <c r="C44" s="186" t="s">
         <v>212</v>
       </c>
-      <c r="D44" s="189" t="s">
-        <v>18</v>
-      </c>
-      <c r="E44" s="191" t="s">
+      <c r="D44" s="188" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="190" t="s">
         <v>214</v>
       </c>
       <c r="F44" s="135" t="s">
         <v>196</v>
       </c>
-      <c r="G44" s="188" t="s">
+      <c r="G44" s="187" t="s">
         <v>197</v>
       </c>
-      <c r="H44" s="281" t="s">
+      <c r="H44" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I44" s="137" t="s">
         <v>543</v>
       </c>
-      <c r="J44" s="193"/>
+      <c r="J44" s="192"/>
     </row>
     <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="334"/>
-      <c r="B45" s="292"/>
+      <c r="A45" s="343"/>
+      <c r="B45" s="358"/>
       <c r="C45" s="164" t="s">
         <v>213</v>
       </c>
-      <c r="D45" s="190" t="s">
+      <c r="D45" s="189" t="s">
         <v>18</v>
       </c>
       <c r="E45" s="163" t="s">
         <v>214</v>
       </c>
-      <c r="F45" s="189" t="s">
+      <c r="F45" s="188" t="s">
         <v>196</v>
       </c>
-      <c r="G45" s="189" t="s">
+      <c r="G45" s="188" t="s">
         <v>197</v>
       </c>
-      <c r="H45" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I45" s="190" t="s">
+      <c r="H45" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I45" s="189" t="s">
         <v>543</v>
       </c>
-      <c r="J45" s="194"/>
+      <c r="J45" s="193"/>
     </row>
     <row r="46" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="334"/>
-      <c r="B46" s="293"/>
-      <c r="C46" s="281" t="s">
+      <c r="A46" s="343"/>
+      <c r="B46" s="338"/>
+      <c r="C46" s="280" t="s">
         <v>366</v>
       </c>
-      <c r="D46" s="283" t="s">
-        <v>18</v>
-      </c>
-      <c r="E46" s="280" t="s">
+      <c r="D46" s="282" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="279" t="s">
         <v>121</v>
       </c>
-      <c r="F46" s="280" t="s">
+      <c r="F46" s="279" t="s">
         <v>532</v>
       </c>
-      <c r="G46" s="281" t="s">
+      <c r="G46" s="280" t="s">
         <v>533</v>
       </c>
-      <c r="H46" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I46" s="281" t="s">
+      <c r="H46" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I46" s="280" t="s">
         <v>542</v>
       </c>
-      <c r="J46" s="282"/>
+      <c r="J46" s="281"/>
     </row>
     <row r="47" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="334"/>
-      <c r="B47" s="291" t="s">
+      <c r="A47" s="343"/>
+      <c r="B47" s="337" t="s">
         <v>144</v>
       </c>
-      <c r="C47" s="336" t="s">
+      <c r="C47" s="345" t="s">
         <v>30</v>
       </c>
       <c r="D47" s="124" t="s">
@@ -5076,7 +5087,7 @@
       <c r="G47" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="H47" s="281" t="s">
+      <c r="H47" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I47" s="138" t="s">
@@ -5085,9 +5096,9 @@
       <c r="J47" s="126"/>
     </row>
     <row r="48" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="334"/>
-      <c r="B48" s="293"/>
-      <c r="C48" s="336"/>
+      <c r="A48" s="343"/>
+      <c r="B48" s="338"/>
+      <c r="C48" s="345"/>
       <c r="D48" s="131" t="s">
         <v>18</v>
       </c>
@@ -5100,7 +5111,7 @@
       <c r="G48" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="H48" s="281" t="s">
+      <c r="H48" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I48" s="133" t="s">
@@ -5109,33 +5120,33 @@
       <c r="J48" s="134"/>
     </row>
     <row r="49" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="334"/>
-      <c r="B49" s="278"/>
-      <c r="C49" s="279"/>
-      <c r="D49" s="280" t="s">
+      <c r="A49" s="343"/>
+      <c r="B49" s="277"/>
+      <c r="C49" s="278"/>
+      <c r="D49" s="279" t="s">
         <v>18</v>
       </c>
       <c r="E49" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="F49" s="280" t="s">
+      <c r="F49" s="279" t="s">
         <v>532</v>
       </c>
-      <c r="G49" s="281" t="s">
+      <c r="G49" s="280" t="s">
         <v>533</v>
       </c>
-      <c r="H49" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I49" s="281" t="s">
+      <c r="H49" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I49" s="280" t="s">
         <v>542</v>
       </c>
-      <c r="J49" s="282"/>
+      <c r="J49" s="281"/>
     </row>
     <row r="50" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="334"/>
-      <c r="B50" s="278"/>
-      <c r="C50" s="168" t="s">
+      <c r="A50" s="343"/>
+      <c r="B50" s="277"/>
+      <c r="C50" s="167" t="s">
         <v>142</v>
       </c>
       <c r="D50" s="135" t="s">
@@ -5150,48 +5161,48 @@
       <c r="G50" s="137" t="s">
         <v>23</v>
       </c>
-      <c r="H50" s="281" t="s">
+      <c r="H50" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I50" s="137" t="s">
         <v>543</v>
       </c>
-      <c r="J50" s="195"/>
+      <c r="J50" s="194"/>
     </row>
     <row r="51" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="335"/>
-      <c r="B51" s="169" t="s">
+      <c r="A51" s="344"/>
+      <c r="B51" s="168" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="168" t="s">
+      <c r="C51" s="167" t="s">
         <v>142</v>
       </c>
-      <c r="D51" s="280" t="s">
-        <v>18</v>
-      </c>
-      <c r="E51" s="280" t="s">
+      <c r="D51" s="279" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" s="279" t="s">
         <v>32</v>
       </c>
-      <c r="F51" s="280" t="s">
+      <c r="F51" s="279" t="s">
         <v>532</v>
       </c>
-      <c r="G51" s="281" t="s">
+      <c r="G51" s="280" t="s">
         <v>533</v>
       </c>
-      <c r="H51" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I51" s="281" t="s">
+      <c r="H51" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I51" s="280" t="s">
         <v>542</v>
       </c>
-      <c r="J51" s="282"/>
+      <c r="J51" s="281"/>
     </row>
     <row r="52" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="28" t="s">
         <v>41</v>
       </c>
       <c r="B52" s="108"/>
-      <c r="C52" s="287" t="s">
+      <c r="C52" s="286" t="s">
         <v>554</v>
       </c>
       <c r="D52" s="22" t="s">
@@ -5206,22 +5217,22 @@
       <c r="G52" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H52" s="281" t="s">
+      <c r="H52" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I52" s="15" t="s">
         <v>542</v>
       </c>
-      <c r="J52" s="198" t="s">
+      <c r="J52" s="197" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="330" t="s">
+      <c r="A53" s="339" t="s">
         <v>36</v>
       </c>
-      <c r="B53" s="173"/>
-      <c r="C53" s="320" t="s">
+      <c r="B53" s="172"/>
+      <c r="C53" s="327" t="s">
         <v>35</v>
       </c>
       <c r="D53" s="63" t="s">
@@ -5236,18 +5247,18 @@
       <c r="G53" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="H53" s="281" t="s">
+      <c r="H53" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I53" s="65" t="s">
         <v>543</v>
       </c>
-      <c r="J53" s="196"/>
+      <c r="J53" s="195"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="331"/>
-      <c r="B54" s="173"/>
-      <c r="C54" s="321"/>
+      <c r="A54" s="340"/>
+      <c r="B54" s="172"/>
+      <c r="C54" s="328"/>
       <c r="D54" s="66" t="s">
         <v>18</v>
       </c>
@@ -5260,18 +5271,18 @@
       <c r="G54" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="H54" s="281" t="s">
+      <c r="H54" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I54" s="68" t="s">
         <v>543</v>
       </c>
-      <c r="J54" s="197"/>
+      <c r="J54" s="196"/>
     </row>
     <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="331"/>
-      <c r="B55" s="173"/>
-      <c r="C55" s="320" t="s">
+      <c r="A55" s="340"/>
+      <c r="B55" s="172"/>
+      <c r="C55" s="327" t="s">
         <v>37</v>
       </c>
       <c r="D55" s="63" t="s">
@@ -5286,18 +5297,18 @@
       <c r="G55" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="H55" s="281" t="s">
+      <c r="H55" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I55" s="65" t="s">
         <v>543</v>
       </c>
-      <c r="J55" s="196"/>
+      <c r="J55" s="195"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="331"/>
-      <c r="B56" s="173"/>
-      <c r="C56" s="321"/>
+      <c r="A56" s="340"/>
+      <c r="B56" s="172"/>
+      <c r="C56" s="328"/>
       <c r="D56" s="66" t="s">
         <v>18</v>
       </c>
@@ -5310,42 +5321,42 @@
       <c r="G56" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="H56" s="281" t="s">
+      <c r="H56" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I56" s="68" t="s">
         <v>543</v>
       </c>
-      <c r="J56" s="197"/>
+      <c r="J56" s="196"/>
     </row>
     <row r="57" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="331"/>
-      <c r="B57" s="209"/>
-      <c r="C57" s="210" t="s">
+      <c r="A57" s="340"/>
+      <c r="B57" s="208"/>
+      <c r="C57" s="209" t="s">
         <v>39</v>
       </c>
-      <c r="D57" s="211" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" s="210" t="s">
+      <c r="D57" s="210" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" s="209" t="s">
         <v>29</v>
       </c>
-      <c r="F57" s="212" t="s">
+      <c r="F57" s="211" t="s">
         <v>15</v>
       </c>
-      <c r="G57" s="213" t="s">
+      <c r="G57" s="212" t="s">
         <v>23</v>
       </c>
-      <c r="H57" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I57" s="213" t="s">
+      <c r="H57" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I57" s="212" t="s">
         <v>543</v>
       </c>
-      <c r="J57" s="214"/>
+      <c r="J57" s="213"/>
     </row>
     <row r="58" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="332"/>
+      <c r="A58" s="341"/>
       <c r="B58" s="109"/>
       <c r="C58" s="70" t="s">
         <v>215</v>
@@ -5362,7 +5373,7 @@
       <c r="G58" s="71" t="s">
         <v>218</v>
       </c>
-      <c r="H58" s="281" t="s">
+      <c r="H58" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I58" s="71" t="s">
@@ -5371,11 +5382,11 @@
       <c r="J58" s="72"/>
     </row>
     <row r="59" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="298" t="s">
+      <c r="A59" s="305" t="s">
         <v>44</v>
       </c>
       <c r="B59" s="110"/>
-      <c r="C59" s="322" t="s">
+      <c r="C59" s="329" t="s">
         <v>42</v>
       </c>
       <c r="D59" s="4" t="s">
@@ -5384,24 +5395,24 @@
       <c r="E59" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F59" s="208" t="s">
+      <c r="F59" s="207" t="s">
         <v>6</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H59" s="281" t="s">
+      <c r="H59" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I59" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="J59" s="199"/>
+      <c r="J59" s="198"/>
     </row>
     <row r="60" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="298"/>
+      <c r="A60" s="305"/>
       <c r="B60" s="110"/>
-      <c r="C60" s="322"/>
+      <c r="C60" s="329"/>
       <c r="D60" s="5" t="s">
         <v>18</v>
       </c>
@@ -5414,7 +5425,7 @@
       <c r="G60" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H60" s="281" t="s">
+      <c r="H60" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I60" s="5" t="s">
@@ -5423,9 +5434,9 @@
       <c r="J60" s="8"/>
     </row>
     <row r="61" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="298"/>
+      <c r="A61" s="305"/>
       <c r="B61" s="110"/>
-      <c r="C61" s="322"/>
+      <c r="C61" s="329"/>
       <c r="D61" s="12" t="s">
         <v>18</v>
       </c>
@@ -5438,7 +5449,7 @@
       <c r="G61" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H61" s="281" t="s">
+      <c r="H61" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I61" s="12" t="s">
@@ -5447,8 +5458,8 @@
       <c r="J61" s="12"/>
     </row>
     <row r="62" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="297"/>
-      <c r="B62" s="174"/>
+      <c r="A62" s="306"/>
+      <c r="B62" s="173"/>
       <c r="C62" s="36" t="s">
         <v>46</v>
       </c>
@@ -5464,7 +5475,7 @@
       <c r="G62" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="H62" s="281" t="s">
+      <c r="H62" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I62" s="42" t="s">
@@ -5473,13 +5484,13 @@
       <c r="J62" s="42"/>
     </row>
     <row r="63" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="353" t="s">
+      <c r="A63" s="297" t="s">
         <v>51</v>
       </c>
       <c r="B63" s="111" t="s">
         <v>49</v>
       </c>
-      <c r="C63" s="172" t="s">
+      <c r="C63" s="171" t="s">
         <v>48</v>
       </c>
       <c r="D63" s="73" t="s">
@@ -5494,7 +5505,7 @@
       <c r="G63" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="H63" s="281" t="s">
+      <c r="H63" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I63" s="73" t="s">
@@ -5505,7 +5516,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="354"/>
+      <c r="A64" s="298"/>
       <c r="B64" s="112" t="s">
         <v>51</v>
       </c>
@@ -5524,7 +5535,7 @@
       <c r="G64" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="H64" s="281" t="s">
+      <c r="H64" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I64" s="75" t="s">
@@ -5538,7 +5549,7 @@
       <c r="A65" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B65" s="175"/>
+      <c r="B65" s="174"/>
       <c r="C65" s="45" t="s">
         <v>54</v>
       </c>
@@ -5554,7 +5565,7 @@
       <c r="G65" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="H65" s="281" t="s">
+      <c r="H65" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I65" s="43" t="s">
@@ -5565,13 +5576,13 @@
       </c>
     </row>
     <row r="66" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="360" t="s">
+      <c r="A66" s="307" t="s">
         <v>149</v>
       </c>
-      <c r="B66" s="365" t="s">
+      <c r="B66" s="312" t="s">
         <v>146</v>
       </c>
-      <c r="C66" s="370" t="s">
+      <c r="C66" s="317" t="s">
         <v>55</v>
       </c>
       <c r="D66" s="57" t="s">
@@ -5586,7 +5597,7 @@
       <c r="G66" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H66" s="281" t="s">
+      <c r="H66" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I66" s="57" t="s">
@@ -5595,9 +5606,9 @@
       <c r="J66" s="57"/>
     </row>
     <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="361"/>
-      <c r="B67" s="366"/>
-      <c r="C67" s="371"/>
+      <c r="A67" s="308"/>
+      <c r="B67" s="313"/>
+      <c r="C67" s="318"/>
       <c r="D67" s="46" t="s">
         <v>18</v>
       </c>
@@ -5610,7 +5621,7 @@
       <c r="G67" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="H67" s="281" t="s">
+      <c r="H67" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I67" s="57" t="s">
@@ -5619,9 +5630,9 @@
       <c r="J67" s="46"/>
     </row>
     <row r="68" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="361"/>
-      <c r="B68" s="366"/>
-      <c r="C68" s="371"/>
+      <c r="A68" s="308"/>
+      <c r="B68" s="313"/>
+      <c r="C68" s="318"/>
       <c r="D68" s="59" t="s">
         <v>18</v>
       </c>
@@ -5634,7 +5645,7 @@
       <c r="G68" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="H68" s="281" t="s">
+      <c r="H68" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I68" s="59" t="s">
@@ -5643,25 +5654,25 @@
       <c r="J68" s="59"/>
     </row>
     <row r="69" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="361"/>
-      <c r="B69" s="367"/>
-      <c r="C69" s="371"/>
+      <c r="A69" s="308"/>
+      <c r="B69" s="314"/>
+      <c r="C69" s="318"/>
       <c r="D69" s="15" t="s">
         <v>18</v>
       </c>
       <c r="E69" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F69" s="190" t="s">
+      <c r="F69" s="189" t="s">
         <v>532</v>
       </c>
       <c r="G69" s="164" t="s">
         <v>534</v>
       </c>
-      <c r="H69" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I69" s="281" t="s">
+      <c r="H69" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I69" s="280" t="s">
         <v>543</v>
       </c>
       <c r="J69" s="22" t="s">
@@ -5669,25 +5680,25 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="361"/>
-      <c r="B70" s="367"/>
-      <c r="C70" s="371"/>
+      <c r="A70" s="308"/>
+      <c r="B70" s="314"/>
+      <c r="C70" s="318"/>
       <c r="D70" s="15" t="s">
         <v>18</v>
       </c>
       <c r="E70" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F70" s="190" t="s">
+      <c r="F70" s="189" t="s">
         <v>536</v>
       </c>
       <c r="G70" s="164" t="s">
         <v>534</v>
       </c>
-      <c r="H70" s="281" t="s">
+      <c r="H70" s="280" t="s">
         <v>547</v>
       </c>
-      <c r="I70" s="281" t="s">
+      <c r="I70" s="280" t="s">
         <v>543</v>
       </c>
       <c r="J70" s="22" t="s">
@@ -5695,25 +5706,25 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="361"/>
-      <c r="B71" s="367"/>
-      <c r="C71" s="371"/>
+      <c r="A71" s="308"/>
+      <c r="B71" s="314"/>
+      <c r="C71" s="318"/>
       <c r="D71" s="15" t="s">
         <v>18</v>
       </c>
       <c r="E71" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F71" s="190" t="s">
+      <c r="F71" s="189" t="s">
         <v>537</v>
       </c>
       <c r="G71" s="164" t="s">
         <v>534</v>
       </c>
-      <c r="H71" s="281" t="s">
+      <c r="H71" s="280" t="s">
         <v>548</v>
       </c>
-      <c r="I71" s="281" t="s">
+      <c r="I71" s="280" t="s">
         <v>543</v>
       </c>
       <c r="J71" s="22" t="s">
@@ -5721,25 +5732,25 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="361"/>
-      <c r="B72" s="367"/>
-      <c r="C72" s="371"/>
+      <c r="A72" s="308"/>
+      <c r="B72" s="314"/>
+      <c r="C72" s="318"/>
       <c r="D72" s="15" t="s">
         <v>18</v>
       </c>
       <c r="E72" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F72" s="190" t="s">
+      <c r="F72" s="189" t="s">
         <v>555</v>
       </c>
       <c r="G72" s="164" t="s">
         <v>534</v>
       </c>
-      <c r="H72" s="281" t="s">
+      <c r="H72" s="280" t="s">
         <v>549</v>
       </c>
-      <c r="I72" s="281" t="s">
+      <c r="I72" s="280" t="s">
         <v>543</v>
       </c>
       <c r="J72" s="22" t="s">
@@ -5747,25 +5758,25 @@
       </c>
     </row>
     <row r="73" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="361"/>
-      <c r="B73" s="367"/>
-      <c r="C73" s="371"/>
+      <c r="A73" s="308"/>
+      <c r="B73" s="314"/>
+      <c r="C73" s="318"/>
       <c r="D73" s="15" t="s">
         <v>18</v>
       </c>
       <c r="E73" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F73" s="190" t="s">
+      <c r="F73" s="189" t="s">
         <v>538</v>
       </c>
       <c r="G73" s="164" t="s">
         <v>534</v>
       </c>
-      <c r="H73" s="281" t="s">
+      <c r="H73" s="280" t="s">
         <v>550</v>
       </c>
-      <c r="I73" s="281" t="s">
+      <c r="I73" s="280" t="s">
         <v>543</v>
       </c>
       <c r="J73" s="22" t="s">
@@ -5773,25 +5784,25 @@
       </c>
     </row>
     <row r="74" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="361"/>
-      <c r="B74" s="367"/>
-      <c r="C74" s="372"/>
+      <c r="A74" s="308"/>
+      <c r="B74" s="314"/>
+      <c r="C74" s="319"/>
       <c r="D74" s="15" t="s">
         <v>18</v>
       </c>
       <c r="E74" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F74" s="190" t="s">
+      <c r="F74" s="189" t="s">
         <v>540</v>
       </c>
       <c r="G74" s="164" t="s">
         <v>534</v>
       </c>
-      <c r="H74" s="281" t="s">
+      <c r="H74" s="280" t="s">
         <v>551</v>
       </c>
-      <c r="I74" s="281" t="s">
+      <c r="I74" s="280" t="s">
         <v>543</v>
       </c>
       <c r="J74" s="22" t="s">
@@ -5799,63 +5810,63 @@
       </c>
     </row>
     <row r="75" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="361"/>
-      <c r="B75" s="367"/>
-      <c r="C75" s="237" t="s">
+      <c r="A75" s="308"/>
+      <c r="B75" s="314"/>
+      <c r="C75" s="236" t="s">
         <v>225</v>
       </c>
-      <c r="D75" s="234" t="s">
-        <v>18</v>
-      </c>
-      <c r="E75" s="234" t="s">
+      <c r="D75" s="233" t="s">
+        <v>18</v>
+      </c>
+      <c r="E75" s="233" t="s">
         <v>45</v>
       </c>
-      <c r="F75" s="234" t="s">
+      <c r="F75" s="233" t="s">
         <v>228</v>
       </c>
-      <c r="G75" s="234" t="s">
+      <c r="G75" s="233" t="s">
         <v>218</v>
       </c>
-      <c r="H75" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I75" s="234" t="s">
+      <c r="H75" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I75" s="233" t="s">
         <v>542</v>
       </c>
-      <c r="J75" s="234"/>
+      <c r="J75" s="233"/>
     </row>
     <row r="76" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="361"/>
-      <c r="B76" s="368"/>
-      <c r="C76" s="237" t="s">
+      <c r="A76" s="308"/>
+      <c r="B76" s="315"/>
+      <c r="C76" s="236" t="s">
         <v>226</v>
       </c>
-      <c r="D76" s="234" t="s">
-        <v>18</v>
-      </c>
-      <c r="E76" s="234" t="s">
+      <c r="D76" s="233" t="s">
+        <v>18</v>
+      </c>
+      <c r="E76" s="233" t="s">
         <v>227</v>
       </c>
-      <c r="F76" s="234" t="s">
+      <c r="F76" s="233" t="s">
         <v>228</v>
       </c>
-      <c r="G76" s="234" t="s">
+      <c r="G76" s="233" t="s">
         <v>218</v>
       </c>
-      <c r="H76" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I76" s="234" t="s">
+      <c r="H76" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I76" s="233" t="s">
         <v>542</v>
       </c>
-      <c r="J76" s="234"/>
+      <c r="J76" s="233"/>
     </row>
     <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="361"/>
-      <c r="B77" s="365" t="s">
+      <c r="A77" s="308"/>
+      <c r="B77" s="312" t="s">
         <v>147</v>
       </c>
-      <c r="C77" s="355" t="s">
+      <c r="C77" s="299" t="s">
         <v>59</v>
       </c>
       <c r="D77" s="57" t="s">
@@ -5870,7 +5881,7 @@
       <c r="G77" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="H77" s="281" t="s">
+      <c r="H77" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I77" s="57" t="s">
@@ -5879,9 +5890,9 @@
       <c r="J77" s="57"/>
     </row>
     <row r="78" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="361"/>
-      <c r="B78" s="366"/>
-      <c r="C78" s="356"/>
+      <c r="A78" s="308"/>
+      <c r="B78" s="313"/>
+      <c r="C78" s="300"/>
       <c r="D78" s="59" t="s">
         <v>18</v>
       </c>
@@ -5894,7 +5905,7 @@
       <c r="G78" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="H78" s="281" t="s">
+      <c r="H78" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I78" s="59" t="s">
@@ -5903,24 +5914,24 @@
       <c r="J78" s="59"/>
     </row>
     <row r="79" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="361"/>
-      <c r="B79" s="366"/>
-      <c r="C79" s="171" t="s">
+      <c r="A79" s="308"/>
+      <c r="B79" s="313"/>
+      <c r="C79" s="170" t="s">
         <v>229</v>
       </c>
-      <c r="D79" s="238" t="s">
-        <v>18</v>
-      </c>
-      <c r="E79" s="239" t="s">
+      <c r="D79" s="237" t="s">
+        <v>18</v>
+      </c>
+      <c r="E79" s="238" t="s">
         <v>29</v>
       </c>
-      <c r="F79" s="241" t="s">
+      <c r="F79" s="240" t="s">
         <v>196</v>
       </c>
       <c r="G79" s="62" t="s">
         <v>218</v>
       </c>
-      <c r="H79" s="281" t="s">
+      <c r="H79" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I79" s="62" t="s">
@@ -5929,40 +5940,40 @@
       <c r="J79" s="62"/>
     </row>
     <row r="80" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="361"/>
-      <c r="B80" s="369"/>
-      <c r="C80" s="171" t="s">
+      <c r="A80" s="308"/>
+      <c r="B80" s="316"/>
+      <c r="C80" s="170" t="s">
         <v>230</v>
       </c>
-      <c r="D80" s="238" t="s">
-        <v>18</v>
-      </c>
-      <c r="E80" s="239" t="s">
+      <c r="D80" s="237" t="s">
+        <v>18</v>
+      </c>
+      <c r="E80" s="238" t="s">
         <v>52</v>
       </c>
-      <c r="F80" s="240" t="s">
+      <c r="F80" s="239" t="s">
         <v>196</v>
       </c>
-      <c r="G80" s="239" t="s">
+      <c r="G80" s="238" t="s">
         <v>218</v>
       </c>
-      <c r="H80" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I80" s="239" t="s">
+      <c r="H80" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I80" s="238" t="s">
         <v>543</v>
       </c>
-      <c r="J80" s="239"/>
+      <c r="J80" s="238"/>
     </row>
     <row r="81" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="361"/>
-      <c r="B81" s="243" t="s">
+      <c r="A81" s="308"/>
+      <c r="B81" s="242" t="s">
         <v>148</v>
       </c>
       <c r="C81" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="D81" s="170" t="s">
+      <c r="D81" s="169" t="s">
         <v>18</v>
       </c>
       <c r="E81" s="62" t="s">
@@ -5974,7 +5985,7 @@
       <c r="G81" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="H81" s="281" t="s">
+      <c r="H81" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I81" s="62" t="s">
@@ -5983,36 +5994,36 @@
       <c r="J81" s="62"/>
     </row>
     <row r="82" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="361"/>
-      <c r="B82" s="244" t="s">
+      <c r="A82" s="308"/>
+      <c r="B82" s="243" t="s">
         <v>168</v>
       </c>
-      <c r="C82" s="176" t="s">
+      <c r="C82" s="175" t="s">
         <v>98</v>
       </c>
-      <c r="D82" s="176" t="s">
-        <v>18</v>
-      </c>
-      <c r="E82" s="176" t="s">
+      <c r="D82" s="175" t="s">
+        <v>18</v>
+      </c>
+      <c r="E82" s="175" t="s">
         <v>99</v>
       </c>
       <c r="F82" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="G82" s="176" t="s">
+      <c r="G82" s="175" t="s">
         <v>23</v>
       </c>
-      <c r="H82" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I82" s="176" t="s">
+      <c r="H82" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I82" s="175" t="s">
         <v>542</v>
       </c>
-      <c r="J82" s="176"/>
+      <c r="J82" s="175"/>
     </row>
     <row r="83" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="361"/>
-      <c r="B83" s="245" t="s">
+      <c r="A83" s="308"/>
+      <c r="B83" s="244" t="s">
         <v>231</v>
       </c>
       <c r="C83" s="62" t="s">
@@ -6024,13 +6035,13 @@
       <c r="E83" s="62" t="s">
         <v>82</v>
       </c>
-      <c r="F83" s="240" t="s">
+      <c r="F83" s="239" t="s">
         <v>196</v>
       </c>
       <c r="G83" s="62" t="s">
         <v>218</v>
       </c>
-      <c r="H83" s="281" t="s">
+      <c r="H83" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I83" s="62" t="s">
@@ -6039,66 +6050,66 @@
       <c r="J83" s="62"/>
     </row>
     <row r="84" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="362"/>
-      <c r="B84" s="242" t="s">
+      <c r="A84" s="309"/>
+      <c r="B84" s="241" t="s">
         <v>235</v>
       </c>
-      <c r="C84" s="238" t="s">
+      <c r="C84" s="237" t="s">
         <v>233</v>
       </c>
-      <c r="D84" s="239" t="s">
-        <v>18</v>
-      </c>
-      <c r="E84" s="239" t="s">
+      <c r="D84" s="238" t="s">
+        <v>18</v>
+      </c>
+      <c r="E84" s="238" t="s">
         <v>234</v>
       </c>
-      <c r="F84" s="240" t="s">
+      <c r="F84" s="239" t="s">
         <v>228</v>
       </c>
-      <c r="G84" s="239" t="s">
+      <c r="G84" s="238" t="s">
         <v>218</v>
       </c>
-      <c r="H84" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I84" s="239" t="s">
+      <c r="H84" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I84" s="238" t="s">
         <v>543</v>
       </c>
-      <c r="J84" s="239"/>
+      <c r="J84" s="238"/>
     </row>
     <row r="85" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="296" t="s">
+      <c r="A85" s="304" t="s">
         <v>151</v>
       </c>
-      <c r="B85" s="236" t="s">
+      <c r="B85" s="235" t="s">
         <v>192</v>
       </c>
-      <c r="C85" s="235" t="s">
+      <c r="C85" s="234" t="s">
         <v>63</v>
       </c>
-      <c r="D85" s="232" t="s">
-        <v>18</v>
-      </c>
-      <c r="E85" s="232" t="s">
+      <c r="D85" s="231" t="s">
+        <v>18</v>
+      </c>
+      <c r="E85" s="231" t="s">
         <v>85</v>
       </c>
-      <c r="F85" s="233" t="s">
+      <c r="F85" s="232" t="s">
         <v>8</v>
       </c>
-      <c r="G85" s="232" t="s">
+      <c r="G85" s="231" t="s">
         <v>9</v>
       </c>
-      <c r="H85" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I85" s="232" t="s">
+      <c r="H85" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I85" s="231" t="s">
         <v>542</v>
       </c>
-      <c r="J85" s="232"/>
+      <c r="J85" s="231"/>
     </row>
     <row r="86" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="298"/>
-      <c r="B86" s="357" t="s">
+      <c r="A86" s="305"/>
+      <c r="B86" s="301" t="s">
         <v>193</v>
       </c>
       <c r="C86" s="42" t="s">
@@ -6116,17 +6127,17 @@
       <c r="G86" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="H86" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I86" s="232" t="s">
+      <c r="H86" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I86" s="231" t="s">
         <v>542</v>
       </c>
       <c r="J86" s="42"/>
     </row>
     <row r="87" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="298"/>
-      <c r="B87" s="358"/>
+      <c r="A87" s="305"/>
+      <c r="B87" s="302"/>
       <c r="C87" s="42" t="s">
         <v>65</v>
       </c>
@@ -6142,17 +6153,17 @@
       <c r="G87" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="H87" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I87" s="232" t="s">
+      <c r="H87" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I87" s="231" t="s">
         <v>542</v>
       </c>
       <c r="J87" s="42"/>
     </row>
     <row r="88" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="298"/>
-      <c r="B88" s="358"/>
+      <c r="A88" s="305"/>
+      <c r="B88" s="302"/>
       <c r="C88" s="42" t="s">
         <v>69</v>
       </c>
@@ -6168,7 +6179,7 @@
       <c r="G88" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="H88" s="281" t="s">
+      <c r="H88" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I88" s="42" t="s">
@@ -6179,8 +6190,8 @@
       </c>
     </row>
     <row r="89" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="298"/>
-      <c r="B89" s="359"/>
+      <c r="A89" s="305"/>
+      <c r="B89" s="303"/>
       <c r="C89" s="42" t="s">
         <v>70</v>
       </c>
@@ -6196,7 +6207,7 @@
       <c r="G89" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="H89" s="281" t="s">
+      <c r="H89" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I89" s="42" t="s">
@@ -6207,8 +6218,8 @@
       </c>
     </row>
     <row r="90" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="297"/>
-      <c r="B90" s="222" t="s">
+      <c r="A90" s="306"/>
+      <c r="B90" s="221" t="s">
         <v>194</v>
       </c>
       <c r="C90" s="22" t="s">
@@ -6226,22 +6237,22 @@
       <c r="G90" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="H90" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I90" s="232" t="s">
+      <c r="H90" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I90" s="231" t="s">
         <v>542</v>
       </c>
       <c r="J90" s="22"/>
     </row>
     <row r="91" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="306" t="s">
+      <c r="A91" s="359" t="s">
         <v>157</v>
       </c>
-      <c r="B91" s="304" t="s">
+      <c r="B91" s="325" t="s">
         <v>152</v>
       </c>
-      <c r="C91" s="302" t="s">
+      <c r="C91" s="323" t="s">
         <v>72</v>
       </c>
       <c r="D91" s="78" t="s">
@@ -6256,7 +6267,7 @@
       <c r="G91" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="H91" s="281" t="s">
+      <c r="H91" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I91" s="78" t="s">
@@ -6267,9 +6278,9 @@
       </c>
     </row>
     <row r="92" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="307"/>
-      <c r="B92" s="305"/>
-      <c r="C92" s="303"/>
+      <c r="A92" s="360"/>
+      <c r="B92" s="326"/>
+      <c r="C92" s="324"/>
       <c r="D92" s="80" t="s">
         <v>18</v>
       </c>
@@ -6282,7 +6293,7 @@
       <c r="G92" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="H92" s="281" t="s">
+      <c r="H92" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I92" s="82" t="s">
@@ -6291,8 +6302,8 @@
       <c r="J92" s="82"/>
     </row>
     <row r="93" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="307"/>
-      <c r="B93" s="220" t="s">
+      <c r="A93" s="360"/>
+      <c r="B93" s="219" t="s">
         <v>153</v>
       </c>
       <c r="C93" s="83" t="s">
@@ -6310,17 +6321,17 @@
       <c r="G93" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="H93" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I93" s="232" t="s">
+      <c r="H93" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I93" s="231" t="s">
         <v>542</v>
       </c>
       <c r="J93" s="83"/>
     </row>
     <row r="94" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="307"/>
-      <c r="B94" s="221" t="s">
+      <c r="A94" s="360"/>
+      <c r="B94" s="220" t="s">
         <v>154</v>
       </c>
       <c r="C94" s="83" t="s">
@@ -6338,17 +6349,17 @@
       <c r="G94" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="H94" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I94" s="232" t="s">
+      <c r="H94" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I94" s="231" t="s">
         <v>542</v>
       </c>
       <c r="J94" s="83"/>
     </row>
     <row r="95" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="307"/>
-      <c r="B95" s="221" t="s">
+      <c r="A95" s="360"/>
+      <c r="B95" s="220" t="s">
         <v>155</v>
       </c>
       <c r="C95" s="83" t="s">
@@ -6366,17 +6377,17 @@
       <c r="G95" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="H95" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I95" s="232" t="s">
+      <c r="H95" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I95" s="231" t="s">
         <v>542</v>
       </c>
       <c r="J95" s="83"/>
     </row>
     <row r="96" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="308"/>
-      <c r="B96" s="221" t="s">
+      <c r="A96" s="361"/>
+      <c r="B96" s="220" t="s">
         <v>156</v>
       </c>
       <c r="C96" s="85" t="s">
@@ -6394,7 +6405,7 @@
       <c r="G96" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="H96" s="281" t="s">
+      <c r="H96" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I96" s="85" t="s">
@@ -6405,10 +6416,10 @@
       </c>
     </row>
     <row r="97" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="296" t="s">
+      <c r="A97" s="304" t="s">
         <v>158</v>
       </c>
-      <c r="B97" s="218" t="s">
+      <c r="B97" s="217" t="s">
         <v>159</v>
       </c>
       <c r="C97" s="36" t="s">
@@ -6426,7 +6437,7 @@
       <c r="G97" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="H97" s="281" t="s">
+      <c r="H97" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I97" s="42" t="s">
@@ -6435,8 +6446,8 @@
       <c r="J97" s="42"/>
     </row>
     <row r="98" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="297"/>
-      <c r="B98" s="219" t="s">
+      <c r="A98" s="306"/>
+      <c r="B98" s="218" t="s">
         <v>160</v>
       </c>
       <c r="C98" s="20" t="s">
@@ -6454,10 +6465,10 @@
       <c r="G98" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="H98" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I98" s="284" t="s">
+      <c r="H98" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I98" s="283" t="s">
         <v>542</v>
       </c>
       <c r="J98" s="17" t="s">
@@ -6465,10 +6476,10 @@
       </c>
     </row>
     <row r="99" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="311" t="s">
+      <c r="A99" s="364" t="s">
         <v>163</v>
       </c>
-      <c r="B99" s="309" t="s">
+      <c r="B99" s="362" t="s">
         <v>161</v>
       </c>
       <c r="C99" s="49" t="s">
@@ -6486,7 +6497,7 @@
       <c r="G99" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="H99" s="281" t="s">
+      <c r="H99" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I99" s="48" t="s">
@@ -6495,8 +6506,8 @@
       <c r="J99" s="48"/>
     </row>
     <row r="100" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A100" s="312"/>
-      <c r="B100" s="310"/>
+      <c r="A100" s="365"/>
+      <c r="B100" s="363"/>
       <c r="C100" s="51" t="s">
         <v>87</v>
       </c>
@@ -6512,7 +6523,7 @@
       <c r="G100" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="H100" s="281" t="s">
+      <c r="H100" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I100" s="50" t="s">
@@ -6523,7 +6534,7 @@
       </c>
     </row>
     <row r="101" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="313"/>
+      <c r="A101" s="366"/>
       <c r="B101" s="114" t="s">
         <v>162</v>
       </c>
@@ -6542,7 +6553,7 @@
       <c r="G101" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="H101" s="281" t="s">
+      <c r="H101" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I101" s="53" t="s">
@@ -6551,11 +6562,11 @@
       <c r="J101" s="53"/>
     </row>
     <row r="102" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="296" t="s">
+      <c r="A102" s="304" t="s">
         <v>164</v>
       </c>
-      <c r="B102" s="178"/>
-      <c r="C102" s="351" t="s">
+      <c r="B102" s="177"/>
+      <c r="C102" s="292" t="s">
         <v>89</v>
       </c>
       <c r="D102" s="39" t="s">
@@ -6570,7 +6581,7 @@
       <c r="G102" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="H102" s="281" t="s">
+      <c r="H102" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I102" s="39" t="s">
@@ -6579,9 +6590,9 @@
       <c r="J102" s="38"/>
     </row>
     <row r="103" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="298"/>
-      <c r="B103" s="179"/>
-      <c r="C103" s="352"/>
+      <c r="A103" s="305"/>
+      <c r="B103" s="178"/>
+      <c r="C103" s="293"/>
       <c r="D103" s="41" t="s">
         <v>18</v>
       </c>
@@ -6594,7 +6605,7 @@
       <c r="G103" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="H103" s="281" t="s">
+      <c r="H103" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I103" s="41" t="s">
@@ -6605,7 +6616,7 @@
       </c>
     </row>
     <row r="104" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="297"/>
+      <c r="A104" s="306"/>
       <c r="B104" s="115"/>
       <c r="C104" s="20" t="s">
         <v>90</v>
@@ -6622,21 +6633,21 @@
       <c r="G104" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="H104" s="281" t="s">
+      <c r="H104" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I104" s="18" t="s">
         <v>542</v>
       </c>
-      <c r="J104" s="201" t="s">
+      <c r="J104" s="200" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="105" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="317" t="s">
+      <c r="A105" s="355" t="s">
         <v>165</v>
       </c>
-      <c r="B105" s="217" t="s">
+      <c r="B105" s="216" t="s">
         <v>95</v>
       </c>
       <c r="C105" s="87" t="s">
@@ -6654,20 +6665,20 @@
       <c r="G105" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="H105" s="281" t="s">
+      <c r="H105" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I105" s="88" t="s">
         <v>542</v>
       </c>
-      <c r="J105" s="200"/>
+      <c r="J105" s="199"/>
     </row>
     <row r="106" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="318"/>
-      <c r="B106" s="217" t="s">
+      <c r="A106" s="356"/>
+      <c r="B106" s="216" t="s">
         <v>167</v>
       </c>
-      <c r="C106" s="177" t="s">
+      <c r="C106" s="176" t="s">
         <v>93</v>
       </c>
       <c r="D106" s="90" t="s">
@@ -6682,17 +6693,17 @@
       <c r="G106" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="H106" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I106" s="232" t="s">
+      <c r="H106" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I106" s="231" t="s">
         <v>542</v>
       </c>
       <c r="J106" s="91"/>
     </row>
     <row r="107" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="319"/>
-      <c r="B107" s="217" t="s">
+      <c r="A107" s="357"/>
+      <c r="B107" s="216" t="s">
         <v>166</v>
       </c>
       <c r="C107" s="87" t="s">
@@ -6710,7 +6721,7 @@
       <c r="G107" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="H107" s="281" t="s">
+      <c r="H107" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I107" s="88" t="s">
@@ -6719,10 +6730,10 @@
       <c r="J107" s="89"/>
     </row>
     <row r="108" spans="1:10" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="288" t="s">
+      <c r="A108" s="294" t="s">
         <v>171</v>
       </c>
-      <c r="B108" s="216" t="s">
+      <c r="B108" s="215" t="s">
         <v>169</v>
       </c>
       <c r="C108" s="36" t="s">
@@ -6740,7 +6751,7 @@
       <c r="G108" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="H108" s="281" t="s">
+      <c r="H108" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I108" s="42" t="s">
@@ -6749,8 +6760,8 @@
       <c r="J108" s="42"/>
     </row>
     <row r="109" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="289"/>
-      <c r="B109" s="181" t="s">
+      <c r="A109" s="295"/>
+      <c r="B109" s="180" t="s">
         <v>170</v>
       </c>
       <c r="C109" s="26" t="s">
@@ -6768,28 +6779,28 @@
       <c r="G109" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="H109" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I109" s="230" t="s">
+      <c r="H109" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I109" s="229" t="s">
         <v>542</v>
       </c>
-      <c r="J109" s="230" t="s">
+      <c r="J109" s="229" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="290"/>
-      <c r="B110" s="227" t="s">
+      <c r="A110" s="296"/>
+      <c r="B110" s="226" t="s">
         <v>220</v>
       </c>
-      <c r="C110" s="228" t="s">
+      <c r="C110" s="227" t="s">
         <v>219</v>
       </c>
-      <c r="D110" s="229" t="s">
-        <v>18</v>
-      </c>
-      <c r="E110" s="201" t="s">
+      <c r="D110" s="228" t="s">
+        <v>18</v>
+      </c>
+      <c r="E110" s="200" t="s">
         <v>56</v>
       </c>
       <c r="F110" s="17" t="s">
@@ -6798,46 +6809,46 @@
       <c r="G110" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="H110" s="281" t="s">
+      <c r="H110" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I110" s="18" t="s">
         <v>542</v>
       </c>
-      <c r="J110" s="201"/>
+      <c r="J110" s="200"/>
     </row>
     <row r="111" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="363" t="s">
+      <c r="A111" s="310" t="s">
         <v>172</v>
       </c>
-      <c r="B111" s="223" t="s">
+      <c r="B111" s="222" t="s">
         <v>173</v>
       </c>
-      <c r="C111" s="224" t="s">
+      <c r="C111" s="223" t="s">
         <v>102</v>
       </c>
-      <c r="D111" s="225" t="s">
-        <v>18</v>
-      </c>
-      <c r="E111" s="226" t="s">
+      <c r="D111" s="224" t="s">
+        <v>18</v>
+      </c>
+      <c r="E111" s="225" t="s">
         <v>104</v>
       </c>
-      <c r="F111" s="226" t="s">
+      <c r="F111" s="225" t="s">
         <v>14</v>
       </c>
-      <c r="G111" s="225" t="s">
+      <c r="G111" s="224" t="s">
         <v>57</v>
       </c>
-      <c r="H111" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I111" s="232" t="s">
+      <c r="H111" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I111" s="231" t="s">
         <v>542</v>
       </c>
-      <c r="J111" s="226"/>
+      <c r="J111" s="225"/>
     </row>
     <row r="112" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="364"/>
+      <c r="A112" s="311"/>
       <c r="B112" s="116" t="s">
         <v>174</v>
       </c>
@@ -6856,16 +6867,16 @@
       <c r="G112" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="H112" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I112" s="232" t="s">
+      <c r="H112" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I112" s="231" t="s">
         <v>542</v>
       </c>
       <c r="J112" s="94"/>
     </row>
     <row r="113" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="296" t="s">
+      <c r="A113" s="304" t="s">
         <v>175</v>
       </c>
       <c r="B113" s="117" t="s">
@@ -6886,7 +6897,7 @@
       <c r="G113" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H113" s="281" t="s">
+      <c r="H113" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I113" s="15" t="s">
@@ -6895,8 +6906,8 @@
       <c r="J113" s="43"/>
     </row>
     <row r="114" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="298"/>
-      <c r="B114" s="182" t="s">
+      <c r="A114" s="305"/>
+      <c r="B114" s="181" t="s">
         <v>110</v>
       </c>
       <c r="C114" s="36" t="s">
@@ -6914,7 +6925,7 @@
       <c r="G114" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="H114" s="281" t="s">
+      <c r="H114" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I114" s="37" t="s">
@@ -6925,8 +6936,8 @@
       </c>
     </row>
     <row r="115" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="297"/>
-      <c r="B115" s="231" t="s">
+      <c r="A115" s="306"/>
+      <c r="B115" s="230" t="s">
         <v>119</v>
       </c>
       <c r="C115" s="26" t="s">
@@ -6944,7 +6955,7 @@
       <c r="G115" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="H115" s="281" t="s">
+      <c r="H115" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I115" s="15" t="s">
@@ -6955,10 +6966,10 @@
       </c>
     </row>
     <row r="116" spans="1:10" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A116" s="288" t="s">
+      <c r="A116" s="294" t="s">
         <v>222</v>
       </c>
-      <c r="B116" s="180" t="s">
+      <c r="B116" s="179" t="s">
         <v>112</v>
       </c>
       <c r="C116" s="36" t="s">
@@ -6976,7 +6987,7 @@
       <c r="G116" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="H116" s="281" t="s">
+      <c r="H116" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I116" s="37" t="s">
@@ -6985,7 +6996,7 @@
       <c r="J116" s="42"/>
     </row>
     <row r="117" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="297"/>
+      <c r="A117" s="306"/>
       <c r="B117" s="113" t="s">
         <v>223</v>
       </c>
@@ -7004,7 +7015,7 @@
       <c r="G117" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="H117" s="281" t="s">
+      <c r="H117" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I117" s="18" t="s">
@@ -7013,37 +7024,37 @@
       <c r="J117" s="17"/>
     </row>
     <row r="118" spans="1:10" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A118" s="296" t="s">
+      <c r="A118" s="304" t="s">
         <v>250</v>
       </c>
-      <c r="B118" s="175" t="s">
+      <c r="B118" s="174" t="s">
         <v>120</v>
       </c>
-      <c r="C118" s="246" t="s">
+      <c r="C118" s="245" t="s">
         <v>113</v>
       </c>
-      <c r="D118" s="246" t="s">
-        <v>18</v>
-      </c>
-      <c r="E118" s="248" t="s">
+      <c r="D118" s="245" t="s">
+        <v>18</v>
+      </c>
+      <c r="E118" s="247" t="s">
         <v>32</v>
       </c>
-      <c r="F118" s="248" t="s">
+      <c r="F118" s="247" t="s">
         <v>12</v>
       </c>
-      <c r="G118" s="247" t="s">
+      <c r="G118" s="246" t="s">
         <v>22</v>
       </c>
-      <c r="H118" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I118" s="247" t="s">
+      <c r="H118" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I118" s="246" t="s">
         <v>542</v>
       </c>
-      <c r="J118" s="248"/>
+      <c r="J118" s="247"/>
     </row>
     <row r="119" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A119" s="297"/>
+      <c r="A119" s="306"/>
       <c r="B119" s="113" t="s">
         <v>251</v>
       </c>
@@ -7062,7 +7073,7 @@
       <c r="G119" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="H119" s="281" t="s">
+      <c r="H119" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I119" s="18" t="s">
@@ -7092,7 +7103,7 @@
       <c r="G120" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H120" s="281" t="s">
+      <c r="H120" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I120" s="14" t="s">
@@ -7101,37 +7112,37 @@
       <c r="J120" s="3"/>
     </row>
     <row r="121" spans="1:10" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A121" s="296" t="s">
+      <c r="A121" s="304" t="s">
         <v>179</v>
       </c>
-      <c r="B121" s="175" t="s">
+      <c r="B121" s="174" t="s">
         <v>239</v>
       </c>
-      <c r="C121" s="246" t="s">
+      <c r="C121" s="245" t="s">
         <v>238</v>
       </c>
-      <c r="D121" s="247" t="s">
-        <v>18</v>
-      </c>
-      <c r="E121" s="248" t="s">
+      <c r="D121" s="246" t="s">
+        <v>18</v>
+      </c>
+      <c r="E121" s="247" t="s">
         <v>217</v>
       </c>
-      <c r="F121" s="248" t="s">
+      <c r="F121" s="247" t="s">
         <v>228</v>
       </c>
-      <c r="G121" s="247" t="s">
+      <c r="G121" s="246" t="s">
         <v>218</v>
       </c>
-      <c r="H121" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I121" s="247" t="s">
+      <c r="H121" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I121" s="246" t="s">
         <v>542</v>
       </c>
-      <c r="J121" s="248"/>
+      <c r="J121" s="247"/>
     </row>
     <row r="122" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A122" s="297"/>
+      <c r="A122" s="306"/>
       <c r="B122" s="113" t="s">
         <v>185</v>
       </c>
@@ -7150,7 +7161,7 @@
       <c r="G122" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H122" s="281" t="s">
+      <c r="H122" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I122" s="18" t="s">
@@ -7180,7 +7191,7 @@
       <c r="G123" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H123" s="281" t="s">
+      <c r="H123" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I123" s="14" t="s">
@@ -7210,7 +7221,7 @@
       <c r="G124" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H124" s="281" t="s">
+      <c r="H124" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I124" s="14" t="s">
@@ -7240,7 +7251,7 @@
       <c r="G125" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H125" s="281" t="s">
+      <c r="H125" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I125" s="14" t="s">
@@ -7272,7 +7283,7 @@
       <c r="G126" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H126" s="281" t="s">
+      <c r="H126" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I126" s="14" t="s">
@@ -7304,7 +7315,7 @@
       <c r="G127" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H127" s="281" t="s">
+      <c r="H127" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I127" s="14" t="s">
@@ -7336,7 +7347,7 @@
       <c r="G128" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="H128" s="281" t="s">
+      <c r="H128" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I128" s="11" t="s">
@@ -7368,7 +7379,7 @@
       <c r="G129" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="H129" s="281" t="s">
+      <c r="H129" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I129" s="44" t="s">
@@ -7377,11 +7388,11 @@
       <c r="J129" s="43"/>
     </row>
     <row r="130" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" s="348" t="s">
+      <c r="A130" s="289" t="s">
         <v>190</v>
       </c>
-      <c r="B130" s="183"/>
-      <c r="C130" s="299" t="s">
+      <c r="B130" s="182"/>
+      <c r="C130" s="320" t="s">
         <v>132</v>
       </c>
       <c r="D130" s="95" t="s">
@@ -7396,7 +7407,7 @@
       <c r="G130" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="H130" s="281" t="s">
+      <c r="H130" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I130" s="95" t="s">
@@ -7407,9 +7418,9 @@
       </c>
     </row>
     <row r="131" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A131" s="349"/>
-      <c r="B131" s="183"/>
-      <c r="C131" s="300"/>
+      <c r="A131" s="290"/>
+      <c r="B131" s="182"/>
+      <c r="C131" s="321"/>
       <c r="D131" s="97" t="s">
         <v>18</v>
       </c>
@@ -7422,7 +7433,7 @@
       <c r="G131" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="H131" s="281" t="s">
+      <c r="H131" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I131" s="95" t="s">
@@ -7433,9 +7444,9 @@
       </c>
     </row>
     <row r="132" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A132" s="349"/>
-      <c r="B132" s="183"/>
-      <c r="C132" s="300"/>
+      <c r="A132" s="290"/>
+      <c r="B132" s="182"/>
+      <c r="C132" s="321"/>
       <c r="D132" s="100" t="s">
         <v>18</v>
       </c>
@@ -7448,7 +7459,7 @@
       <c r="G132" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="H132" s="281" t="s">
+      <c r="H132" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I132" s="95" t="s">
@@ -7459,9 +7470,9 @@
       </c>
     </row>
     <row r="133" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A133" s="349"/>
-      <c r="B133" s="184"/>
-      <c r="C133" s="300"/>
+      <c r="A133" s="290"/>
+      <c r="B133" s="183"/>
+      <c r="C133" s="321"/>
       <c r="D133" s="100" t="s">
         <v>18</v>
       </c>
@@ -7474,7 +7485,7 @@
       <c r="G133" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="H133" s="281" t="s">
+      <c r="H133" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I133" s="95" t="s">
@@ -7485,9 +7496,9 @@
       </c>
     </row>
     <row r="134" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A134" s="349"/>
-      <c r="B134" s="185"/>
-      <c r="C134" s="301"/>
+      <c r="A134" s="290"/>
+      <c r="B134" s="184"/>
+      <c r="C134" s="322"/>
       <c r="D134" s="101" t="s">
         <v>18</v>
       </c>
@@ -7500,7 +7511,7 @@
       <c r="G134" s="101" t="s">
         <v>150</v>
       </c>
-      <c r="H134" s="281" t="s">
+      <c r="H134" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I134" s="95" t="s">
@@ -7511,9 +7522,9 @@
       </c>
     </row>
     <row r="135" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A135" s="349"/>
-      <c r="B135" s="185"/>
-      <c r="C135" s="346" t="s">
+      <c r="A135" s="290"/>
+      <c r="B135" s="184"/>
+      <c r="C135" s="287" t="s">
         <v>137</v>
       </c>
       <c r="D135" s="103" t="s">
@@ -7528,7 +7539,7 @@
       <c r="G135" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="H135" s="281" t="s">
+      <c r="H135" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I135" s="95" t="s">
@@ -7539,9 +7550,9 @@
       </c>
     </row>
     <row r="136" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A136" s="349"/>
-      <c r="B136" s="185"/>
-      <c r="C136" s="347"/>
+      <c r="A136" s="290"/>
+      <c r="B136" s="184"/>
+      <c r="C136" s="288"/>
       <c r="D136" s="105" t="s">
         <v>18</v>
       </c>
@@ -7554,7 +7565,7 @@
       <c r="G136" s="105" t="s">
         <v>150</v>
       </c>
-      <c r="H136" s="281" t="s">
+      <c r="H136" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I136" s="95" t="s">
@@ -7565,9 +7576,9 @@
       </c>
     </row>
     <row r="137" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A137" s="350"/>
-      <c r="B137" s="186"/>
-      <c r="C137" s="215" t="s">
+      <c r="A137" s="291"/>
+      <c r="B137" s="185"/>
+      <c r="C137" s="214" t="s">
         <v>139</v>
       </c>
       <c r="D137" s="144" t="s">
@@ -7582,7 +7593,7 @@
       <c r="G137" s="146" t="s">
         <v>150</v>
       </c>
-      <c r="H137" s="281" t="s">
+      <c r="H137" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I137" s="95" t="s">
@@ -7593,7 +7604,7 @@
       </c>
     </row>
     <row r="138" spans="1:10" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="314" t="s">
+      <c r="A138" s="369" t="s">
         <v>198</v>
       </c>
       <c r="B138" s="149"/>
@@ -7612,7 +7623,7 @@
       <c r="G138" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="H138" s="281" t="s">
+      <c r="H138" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I138" s="19" t="s">
@@ -7621,7 +7632,7 @@
       <c r="J138" s="19"/>
     </row>
     <row r="139" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="315"/>
+      <c r="A139" s="370"/>
       <c r="B139" s="150"/>
       <c r="C139" s="2" t="s">
         <v>200</v>
@@ -7638,7 +7649,7 @@
       <c r="G139" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="H139" s="281" t="s">
+      <c r="H139" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I139" s="2" t="s">
@@ -7647,7 +7658,7 @@
       <c r="J139" s="2"/>
     </row>
     <row r="140" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A140" s="316"/>
+      <c r="A140" s="371"/>
       <c r="B140" s="152"/>
       <c r="C140" s="25" t="s">
         <v>261</v>
@@ -7664,7 +7675,7 @@
       <c r="G140" s="25" t="s">
         <v>254</v>
       </c>
-      <c r="H140" s="281" t="s">
+      <c r="H140" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I140" s="25" t="s">
@@ -7673,7 +7684,7 @@
       <c r="J140" s="25"/>
     </row>
     <row r="141" spans="1:10" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="314" t="s">
+      <c r="A141" s="369" t="s">
         <v>206</v>
       </c>
       <c r="B141" s="149"/>
@@ -7692,7 +7703,7 @@
       <c r="G141" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="H141" s="281" t="s">
+      <c r="H141" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I141" s="25" t="s">
@@ -7701,7 +7712,7 @@
       <c r="J141" s="19"/>
     </row>
     <row r="142" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="315"/>
+      <c r="A142" s="370"/>
       <c r="B142" s="150"/>
       <c r="C142" s="154" t="s">
         <v>204</v>
@@ -7718,7 +7729,7 @@
       <c r="G142" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="H142" s="281" t="s">
+      <c r="H142" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I142" s="25" t="s">
@@ -7727,7 +7738,7 @@
       <c r="J142" s="2"/>
     </row>
     <row r="143" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A143" s="316"/>
+      <c r="A143" s="371"/>
       <c r="B143" s="151"/>
       <c r="C143" s="148" t="s">
         <v>205</v>
@@ -7744,7 +7755,7 @@
       <c r="G143" s="147" t="s">
         <v>197</v>
       </c>
-      <c r="H143" s="281" t="s">
+      <c r="H143" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I143" s="25" t="s">
@@ -7772,7 +7783,7 @@
       <c r="G144" s="147" t="s">
         <v>197</v>
       </c>
-      <c r="H144" s="281" t="s">
+      <c r="H144" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I144" s="25" t="s">
@@ -7800,7 +7811,7 @@
       <c r="G145" s="147" t="s">
         <v>197</v>
       </c>
-      <c r="H145" s="281" t="s">
+      <c r="H145" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I145" s="25" t="s">
@@ -7828,7 +7839,7 @@
       <c r="G146" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="H146" s="281" t="s">
+      <c r="H146" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I146" s="6" t="s">
@@ -7837,38 +7848,38 @@
       <c r="J146" s="6"/>
     </row>
     <row r="147" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A147" s="294" t="s">
+      <c r="A147" s="367" t="s">
         <v>240</v>
       </c>
-      <c r="B147" s="249" t="s">
+      <c r="B147" s="248" t="s">
         <v>265</v>
       </c>
-      <c r="C147" s="248" t="s">
+      <c r="C147" s="247" t="s">
         <v>262</v>
       </c>
-      <c r="D147" s="246" t="s">
-        <v>18</v>
-      </c>
-      <c r="E147" s="246" t="s">
+      <c r="D147" s="245" t="s">
+        <v>18</v>
+      </c>
+      <c r="E147" s="245" t="s">
         <v>264</v>
       </c>
-      <c r="F147" s="246" t="s">
+      <c r="F147" s="245" t="s">
         <v>228</v>
       </c>
-      <c r="G147" s="246" t="s">
+      <c r="G147" s="245" t="s">
         <v>254</v>
       </c>
-      <c r="H147" s="281" t="s">
-        <v>546</v>
-      </c>
-      <c r="I147" s="246" t="s">
+      <c r="H147" s="280" t="s">
+        <v>546</v>
+      </c>
+      <c r="I147" s="245" t="s">
         <v>542</v>
       </c>
-      <c r="J147" s="246"/>
+      <c r="J147" s="245"/>
     </row>
     <row r="148" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A148" s="295"/>
-      <c r="B148" s="250" t="s">
+      <c r="A148" s="368"/>
+      <c r="B148" s="249" t="s">
         <v>266</v>
       </c>
       <c r="C148" s="17" t="s">
@@ -7886,7 +7897,7 @@
       <c r="G148" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="H148" s="281" t="s">
+      <c r="H148" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I148" s="20" t="s">
@@ -7914,7 +7925,7 @@
       <c r="G149" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="H149" s="281" t="s">
+      <c r="H149" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I149" s="20" t="s">
@@ -7942,7 +7953,7 @@
       <c r="G150" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="H150" s="281" t="s">
+      <c r="H150" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I150" s="20" t="s">
@@ -7970,7 +7981,7 @@
       <c r="G151" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="H151" s="281" t="s">
+      <c r="H151" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I151" s="20" t="s">
@@ -7998,7 +8009,7 @@
       <c r="G152" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="H152" s="281" t="s">
+      <c r="H152" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I152" s="20" t="s">
@@ -8026,7 +8037,7 @@
       <c r="G153" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="H153" s="281" t="s">
+      <c r="H153" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I153" s="20" t="s">
@@ -8054,7 +8065,7 @@
       <c r="G154" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="H154" s="281" t="s">
+      <c r="H154" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I154" s="20" t="s">
@@ -8082,7 +8093,7 @@
       <c r="G155" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="H155" s="281" t="s">
+      <c r="H155" s="280" t="s">
         <v>546</v>
       </c>
       <c r="I155" s="20" t="s">
@@ -9136,6 +9147,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A113:A115"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A138:A140"/>
+    <mergeCell ref="A105:A107"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A2:A27"/>
+    <mergeCell ref="B28:B46"/>
+    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A28:A51"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C28:C41"/>
+    <mergeCell ref="C12:C23"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="B12:B27"/>
     <mergeCell ref="C135:C136"/>
     <mergeCell ref="A130:A137"/>
     <mergeCell ref="C102:C103"/>
@@ -9149,37 +9188,9 @@
     <mergeCell ref="B66:B76"/>
     <mergeCell ref="B77:B80"/>
     <mergeCell ref="C66:C74"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="B2:B11"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A53:A58"/>
-    <mergeCell ref="A28:A51"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C28:C41"/>
-    <mergeCell ref="C12:C23"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="B12:B27"/>
     <mergeCell ref="C130:C134"/>
     <mergeCell ref="C91:C92"/>
     <mergeCell ref="B91:B92"/>
-    <mergeCell ref="A91:A96"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="A105:A107"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A2:A27"/>
-    <mergeCell ref="B28:B46"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A113:A115"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A138:A140"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9197,187 +9208,187 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" style="253" customWidth="1"/>
+    <col min="1" max="1" width="28.54296875" style="252" customWidth="1"/>
     <col min="2" max="2" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.453125" style="253" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" style="252" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="254" t="s">
+      <c r="A1" s="253" t="s">
         <v>347</v>
       </c>
-      <c r="B1" s="254" t="s">
+      <c r="B1" s="253" t="s">
         <v>368</v>
       </c>
-      <c r="C1" s="254" t="s">
+      <c r="C1" s="253" t="s">
         <v>351</v>
       </c>
-      <c r="D1" s="253" t="s">
+      <c r="D1" s="252" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="255" t="s">
+      <c r="A2" s="254" t="s">
         <v>339</v>
       </c>
-      <c r="B2" s="255" t="s">
+      <c r="B2" s="254" t="s">
         <v>339</v>
       </c>
       <c r="C2" s="27"/>
-      <c r="D2" s="261"/>
+      <c r="D2" s="260"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="255" t="s">
+      <c r="A3" s="254" t="s">
         <v>340</v>
       </c>
-      <c r="B3" s="255" t="s">
+      <c r="B3" s="254" t="s">
         <v>340</v>
       </c>
       <c r="C3" s="27"/>
-      <c r="D3" s="261"/>
+      <c r="D3" s="260"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="255" t="s">
+      <c r="A4" s="254" t="s">
         <v>345</v>
       </c>
-      <c r="B4" s="255" t="s">
+      <c r="B4" s="254" t="s">
         <v>345</v>
       </c>
       <c r="C4" s="27"/>
-      <c r="D4" s="261"/>
+      <c r="D4" s="260"/>
     </row>
     <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="263" t="s">
+      <c r="A5" s="262" t="s">
         <v>348</v>
       </c>
-      <c r="B5" s="263" t="s">
+      <c r="B5" s="262" t="s">
         <v>348</v>
       </c>
       <c r="C5" s="27"/>
-      <c r="D5" s="261" t="s">
+      <c r="D5" s="260" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="255" t="s">
+      <c r="A6" s="254" t="s">
         <v>354</v>
       </c>
-      <c r="B6" s="255" t="s">
+      <c r="B6" s="254" t="s">
         <v>354</v>
       </c>
-      <c r="C6" s="259" t="s">
+      <c r="C6" s="258" t="s">
         <v>353</v>
       </c>
-      <c r="D6" s="261" t="s">
+      <c r="D6" s="260" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="255" t="s">
+      <c r="A7" s="254" t="s">
         <v>369</v>
       </c>
-      <c r="B7" s="255" t="s">
+      <c r="B7" s="254" t="s">
         <v>369</v>
       </c>
-      <c r="C7" s="258" t="s">
+      <c r="C7" s="257" t="s">
         <v>349</v>
       </c>
-      <c r="D7" s="261" t="s">
+      <c r="D7" s="260" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="255" t="s">
+      <c r="A8" s="254" t="s">
         <v>344</v>
       </c>
-      <c r="B8" s="255" t="s">
+      <c r="B8" s="254" t="s">
         <v>344</v>
       </c>
-      <c r="C8" s="259"/>
-      <c r="D8" s="261"/>
+      <c r="C8" s="258"/>
+      <c r="D8" s="260"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="255" t="s">
+      <c r="A9" s="254" t="s">
         <v>343</v>
       </c>
-      <c r="B9" s="255" t="s">
+      <c r="B9" s="254" t="s">
         <v>343</v>
       </c>
-      <c r="C9" s="259"/>
-      <c r="D9" s="261"/>
+      <c r="C9" s="258"/>
+      <c r="D9" s="260"/>
     </row>
     <row r="10" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="264" t="s">
+      <c r="A10" s="263" t="s">
         <v>342</v>
       </c>
-      <c r="B10" s="264" t="s">
+      <c r="B10" s="263" t="s">
         <v>342</v>
       </c>
-      <c r="C10" s="259"/>
-      <c r="D10" s="266" t="s">
+      <c r="C10" s="258"/>
+      <c r="D10" s="265" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A11" s="265" t="s">
+      <c r="A11" s="264" t="s">
         <v>350</v>
       </c>
-      <c r="B11" s="265" t="s">
+      <c r="B11" s="264" t="s">
         <v>350</v>
       </c>
       <c r="C11" s="27"/>
-      <c r="D11" s="266" t="s">
+      <c r="D11" s="265" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="257" t="s">
+      <c r="A12" s="256" t="s">
         <v>346</v>
       </c>
-      <c r="B12" s="257" t="s">
+      <c r="B12" s="256" t="s">
         <v>346</v>
       </c>
-      <c r="C12" s="259"/>
-      <c r="D12" s="261"/>
+      <c r="C12" s="258"/>
+      <c r="D12" s="260"/>
     </row>
     <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="255" t="s">
+      <c r="A13" s="254" t="s">
         <v>341</v>
       </c>
-      <c r="B13" s="255" t="s">
+      <c r="B13" s="254" t="s">
         <v>341</v>
       </c>
-      <c r="C13" s="258" t="s">
+      <c r="C13" s="257" t="s">
         <v>341</v>
       </c>
-      <c r="D13" s="261" t="s">
+      <c r="D13" s="260" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="256" t="s">
+      <c r="A14" s="255" t="s">
         <v>352</v>
       </c>
-      <c r="B14" s="256" t="s">
+      <c r="B14" s="255" t="s">
         <v>352</v>
       </c>
-      <c r="C14" s="259"/>
-      <c r="D14" s="262" t="s">
+      <c r="C14" s="258"/>
+      <c r="D14" s="261" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A15" s="256" t="s">
+      <c r="A15" s="255" t="s">
         <v>357</v>
       </c>
-      <c r="B15" s="256" t="s">
+      <c r="B15" s="255" t="s">
         <v>357</v>
       </c>
-      <c r="C15" s="260" t="s">
+      <c r="C15" s="259" t="s">
         <v>358</v>
       </c>
-      <c r="D15" s="261" t="s">
+      <c r="D15" s="260" t="s">
         <v>362</v>
       </c>
     </row>
@@ -9419,12 +9430,12 @@
       <c r="A2" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="251" t="s">
+      <c r="B2" s="250" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="235" t="s">
+      <c r="A3" s="234" t="s">
         <v>232</v>
       </c>
       <c r="B3" t="s">
@@ -9467,7 +9478,7 @@
       <c r="A8" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="B8" s="251" t="s">
+      <c r="B8" s="250" t="s">
         <v>284</v>
       </c>
     </row>
@@ -9531,7 +9542,7 @@
       <c r="A16" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="B16" s="251" t="s">
+      <c r="B16" s="250" t="s">
         <v>367</v>
       </c>
     </row>
@@ -9552,10 +9563,10 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="246" t="s">
+      <c r="A19" s="245" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="267" t="s">
+      <c r="B19" s="266" t="s">
         <v>363</v>
       </c>
     </row>
@@ -9563,7 +9574,7 @@
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="252" t="s">
+      <c r="B20" s="251" t="s">
         <v>365</v>
       </c>
     </row>
@@ -9587,7 +9598,7 @@
       <c r="A23" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="251" t="s">
+      <c r="B23" s="250" t="s">
         <v>270</v>
       </c>
     </row>
@@ -9600,10 +9611,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="268" t="s">
+      <c r="A25" s="267" t="s">
         <v>102</v>
       </c>
-      <c r="B25" s="251" t="s">
+      <c r="B25" s="250" t="s">
         <v>274</v>
       </c>
     </row>
@@ -9632,26 +9643,26 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="268" t="s">
+      <c r="A29" s="267" t="s">
         <v>142</v>
       </c>
-      <c r="B29" s="267" t="s">
+      <c r="B29" s="266" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="268" t="s">
+      <c r="A30" s="267" t="s">
         <v>142</v>
       </c>
-      <c r="B30" s="251" t="s">
+      <c r="B30" s="250" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="268" t="s">
+      <c r="A31" s="267" t="s">
         <v>210</v>
       </c>
-      <c r="B31" s="251" t="s">
+      <c r="B31" s="250" t="s">
         <v>280</v>
       </c>
     </row>
@@ -9659,7 +9670,7 @@
       <c r="A32" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B32" s="252" t="s">
+      <c r="B32" s="251" t="s">
         <v>285</v>
       </c>
     </row>
@@ -9667,7 +9678,7 @@
       <c r="A33" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="B33" s="251" t="s">
+      <c r="B33" s="250" t="s">
         <v>282</v>
       </c>
     </row>
@@ -9707,7 +9718,7 @@
       <c r="A38" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="251" t="s">
+      <c r="B38" s="250" t="s">
         <v>271</v>
       </c>
     </row>
@@ -9752,10 +9763,10 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="268" t="s">
+      <c r="A44" s="267" t="s">
         <v>208</v>
       </c>
-      <c r="B44" s="251" t="s">
+      <c r="B44" s="250" t="s">
         <v>279</v>
       </c>
     </row>
@@ -9795,7 +9806,7 @@
       <c r="A49" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="251" t="s">
+      <c r="B49" s="250" t="s">
         <v>552</v>
       </c>
     </row>
@@ -9811,7 +9822,7 @@
       <c r="A51" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B51" s="251" t="s">
+      <c r="B51" s="250" t="s">
         <v>268</v>
       </c>
     </row>
@@ -9851,7 +9862,7 @@
       <c r="A56" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="251" t="s">
+      <c r="B56" s="250" t="s">
         <v>553</v>
       </c>
     </row>
@@ -9912,10 +9923,10 @@
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="268" t="s">
+      <c r="A64" s="267" t="s">
         <v>94</v>
       </c>
-      <c r="B64" s="251" t="s">
+      <c r="B64" s="250" t="s">
         <v>272</v>
       </c>
     </row>
@@ -9931,7 +9942,7 @@
       <c r="A66" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="251" t="s">
+      <c r="B66" s="250" t="s">
         <v>273</v>
       </c>
     </row>
@@ -9952,18 +9963,18 @@
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="268" t="s">
+      <c r="A69" s="267" t="s">
         <v>87</v>
       </c>
-      <c r="B69" s="251" t="s">
+      <c r="B69" s="250" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="268" t="s">
+      <c r="A70" s="267" t="s">
         <v>122</v>
       </c>
-      <c r="B70" s="251" t="s">
+      <c r="B70" s="250" t="s">
         <v>277</v>
       </c>
     </row>
@@ -10019,7 +10030,7 @@
       <c r="A77" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B77" s="251" t="s">
+      <c r="B77" s="250" t="s">
         <v>275</v>
       </c>
     </row>
@@ -10059,7 +10070,7 @@
       <c r="A82" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="B82" s="251" t="s">
+      <c r="B82" s="250" t="s">
         <v>283</v>
       </c>
     </row>
@@ -10067,7 +10078,7 @@
       <c r="A83" s="43" t="s">
         <v>221</v>
       </c>
-      <c r="B83" s="251" t="s">
+      <c r="B83" s="250" t="s">
         <v>281</v>
       </c>
     </row>
@@ -10075,7 +10086,7 @@
       <c r="A84" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="B84" s="251" t="s">
+      <c r="B84" s="250" t="s">
         <v>33</v>
       </c>
     </row>
@@ -10083,7 +10094,7 @@
       <c r="A85" s="43" t="s">
         <v>554</v>
       </c>
-      <c r="B85" s="251" t="s">
+      <c r="B85" s="250" t="s">
         <v>371</v>
       </c>
     </row>
@@ -10091,15 +10102,15 @@
       <c r="A86" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="B86" s="251" t="s">
+      <c r="B86" s="250" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" s="172" t="s">
+      <c r="A87" s="171" t="s">
         <v>48</v>
       </c>
-      <c r="B87" s="251" t="s">
+      <c r="B87" s="250" t="s">
         <v>373</v>
       </c>
     </row>
@@ -10107,7 +10118,7 @@
       <c r="A88" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="B88" s="251" t="s">
+      <c r="B88" s="250" t="s">
         <v>374</v>
       </c>
     </row>
@@ -10115,7 +10126,7 @@
       <c r="A89" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="B89" s="251" t="s">
+      <c r="B89" s="250" t="s">
         <v>375</v>
       </c>
     </row>
@@ -10123,7 +10134,7 @@
       <c r="A90" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B90" s="251" t="s">
+      <c r="B90" s="250" t="s">
         <v>376</v>
       </c>
     </row>
@@ -10131,7 +10142,7 @@
       <c r="A91" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B91" s="251" t="s">
+      <c r="B91" s="250" t="s">
         <v>83</v>
       </c>
     </row>
@@ -10139,7 +10150,7 @@
       <c r="A92" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B92" s="251" t="s">
+      <c r="B92" s="250" t="s">
         <v>377</v>
       </c>
     </row>
@@ -10147,7 +10158,7 @@
       <c r="A93" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B93" s="251" t="s">
+      <c r="B93" s="250" t="s">
         <v>378</v>
       </c>
     </row>
@@ -10155,7 +10166,7 @@
       <c r="A94" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B94" s="251" t="s">
+      <c r="B94" s="250" t="s">
         <v>379</v>
       </c>
     </row>
@@ -10163,15 +10174,15 @@
       <c r="A95" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="B95" s="251" t="s">
+      <c r="B95" s="250" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" s="215" t="s">
+      <c r="A96" s="214" t="s">
         <v>139</v>
       </c>
-      <c r="B96" s="251" t="s">
+      <c r="B96" s="250" t="s">
         <v>139</v>
       </c>
     </row>
@@ -10179,7 +10190,7 @@
       <c r="A97" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="B97" s="251" t="s">
+      <c r="B97" s="250" t="s">
         <v>381</v>
       </c>
     </row>
@@ -10187,7 +10198,7 @@
       <c r="A98" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="B98" s="251" t="s">
+      <c r="B98" s="250" t="s">
         <v>382</v>
       </c>
     </row>
@@ -10195,7 +10206,7 @@
       <c r="A99" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B99" s="252" t="s">
+      <c r="B99" s="251" t="s">
         <v>383</v>
       </c>
     </row>
@@ -10267,7 +10278,7 @@
       <c r="A6" t="s">
         <v>390</v>
       </c>
-      <c r="B6" s="272" t="s">
+      <c r="B6" s="271" t="s">
         <v>418</v>
       </c>
     </row>
@@ -10275,7 +10286,7 @@
       <c r="A7" t="s">
         <v>391</v>
       </c>
-      <c r="B7" s="272" t="s">
+      <c r="B7" s="271" t="s">
         <v>423</v>
       </c>
     </row>
@@ -10283,7 +10294,7 @@
       <c r="A8" t="s">
         <v>392</v>
       </c>
-      <c r="B8" s="272" t="s">
+      <c r="B8" s="271" t="s">
         <v>424</v>
       </c>
     </row>
@@ -10291,7 +10302,7 @@
       <c r="A9" t="s">
         <v>393</v>
       </c>
-      <c r="B9" s="272" t="s">
+      <c r="B9" s="271" t="s">
         <v>425</v>
       </c>
     </row>
@@ -10299,7 +10310,7 @@
       <c r="A10" t="s">
         <v>394</v>
       </c>
-      <c r="B10" s="272" t="s">
+      <c r="B10" s="271" t="s">
         <v>419</v>
       </c>
     </row>
@@ -10307,7 +10318,7 @@
       <c r="A11" t="s">
         <v>395</v>
       </c>
-      <c r="B11" s="272" t="s">
+      <c r="B11" s="271" t="s">
         <v>420</v>
       </c>
     </row>
@@ -10315,7 +10326,7 @@
       <c r="A12" t="s">
         <v>396</v>
       </c>
-      <c r="B12" s="272" t="s">
+      <c r="B12" s="271" t="s">
         <v>421</v>
       </c>
     </row>
@@ -10323,7 +10334,7 @@
       <c r="A13" t="s">
         <v>397</v>
       </c>
-      <c r="B13" s="272" t="s">
+      <c r="B13" s="271" t="s">
         <v>422</v>
       </c>
     </row>
@@ -10331,7 +10342,7 @@
       <c r="A14" t="s">
         <v>398</v>
       </c>
-      <c r="B14" s="273" t="s">
+      <c r="B14" s="272" t="s">
         <v>414</v>
       </c>
     </row>
@@ -10339,7 +10350,7 @@
       <c r="A15" t="s">
         <v>399</v>
       </c>
-      <c r="B15" s="273" t="s">
+      <c r="B15" s="272" t="s">
         <v>415</v>
       </c>
     </row>
@@ -10347,7 +10358,7 @@
       <c r="A16" t="s">
         <v>400</v>
       </c>
-      <c r="B16" s="273" t="s">
+      <c r="B16" s="272" t="s">
         <v>416</v>
       </c>
     </row>
@@ -10355,7 +10366,7 @@
       <c r="A17" t="s">
         <v>401</v>
       </c>
-      <c r="B17" s="273" t="s">
+      <c r="B17" s="272" t="s">
         <v>417</v>
       </c>
     </row>
@@ -10363,7 +10374,7 @@
       <c r="A18" t="s">
         <v>402</v>
       </c>
-      <c r="B18" s="272" t="s">
+      <c r="B18" s="271" t="s">
         <v>410</v>
       </c>
     </row>
@@ -10371,7 +10382,7 @@
       <c r="A19" t="s">
         <v>403</v>
       </c>
-      <c r="B19" s="272" t="s">
+      <c r="B19" s="271" t="s">
         <v>411</v>
       </c>
     </row>
@@ -10379,7 +10390,7 @@
       <c r="A20" t="s">
         <v>404</v>
       </c>
-      <c r="B20" s="272" t="s">
+      <c r="B20" s="271" t="s">
         <v>412</v>
       </c>
     </row>
@@ -10387,7 +10398,7 @@
       <c r="A21" t="s">
         <v>405</v>
       </c>
-      <c r="B21" s="272" t="s">
+      <c r="B21" s="271" t="s">
         <v>413</v>
       </c>
     </row>
@@ -10395,7 +10406,7 @@
       <c r="A22" t="s">
         <v>406</v>
       </c>
-      <c r="B22" s="270" t="s">
+      <c r="B22" s="269" t="s">
         <v>409</v>
       </c>
     </row>
@@ -10403,7 +10414,7 @@
       <c r="A23" t="s">
         <v>407</v>
       </c>
-      <c r="B23" s="271" t="s">
+      <c r="B23" s="270" t="s">
         <v>408</v>
       </c>
     </row>
@@ -10442,7 +10453,7 @@
       <c r="A2" t="s">
         <v>430</v>
       </c>
-      <c r="B2" s="269" t="s">
+      <c r="B2" s="268" t="s">
         <v>528</v>
       </c>
     </row>
@@ -10450,7 +10461,7 @@
       <c r="A3" t="s">
         <v>431</v>
       </c>
-      <c r="B3" s="269" t="s">
+      <c r="B3" s="268" t="s">
         <v>529</v>
       </c>
     </row>
@@ -10458,7 +10469,7 @@
       <c r="A4" t="s">
         <v>432</v>
       </c>
-      <c r="B4" s="269" t="s">
+      <c r="B4" s="268" t="s">
         <v>530</v>
       </c>
     </row>
@@ -10466,7 +10477,7 @@
       <c r="A5" t="s">
         <v>433</v>
       </c>
-      <c r="B5" s="269" t="s">
+      <c r="B5" s="268" t="s">
         <v>531</v>
       </c>
     </row>

</xml_diff>